<commit_message>
Beginning of status affliction code
</commit_message>
<xml_diff>
--- a/FFL2 Data.xlsx
+++ b/FFL2 Data.xlsx
@@ -932,7 +932,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10902" uniqueCount="3461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10902" uniqueCount="3462">
   <si>
     <t>Monster</t>
   </si>
@@ -11326,6 +11326,9 @@
   </si>
   <si>
     <t>Damage=target.maxHP * 10 / attacker.initiative + 2; one group</t>
+  </si>
+  <si>
+    <t>All enemies; Stun</t>
   </si>
 </sst>
 </file>
@@ -38655,9 +38658,9 @@
   <sheetPr codeName="Sheet4" filterMode="1"/>
   <dimension ref="A1:Y213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W48" sqref="W48"/>
+      <selection pane="bottomLeft" activeCell="P214" sqref="P214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38785,7 +38788,7 @@
         <v>1877</v>
       </c>
       <c r="P2" t="s">
-        <v>3381</v>
+        <v>5</v>
       </c>
       <c r="Q2">
         <v>11</v>
@@ -40169,7 +40172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" hidden="1">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Heal Staff</v>
@@ -41182,7 +41185,7 @@
         <v>3449</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" hidden="1">
       <c r="A48" t="s">
         <v>3452</v>
       </c>
@@ -42335,7 +42338,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:25" hidden="1">
+    <row r="67" spans="1:25">
       <c r="A67" t="str">
         <f t="shared" si="7"/>
         <v>Temptat</v>
@@ -42386,14 +42389,14 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="68" spans="1:25" hidden="1">
+    <row r="68" spans="1:25">
       <c r="A68" t="str">
         <f t="shared" si="7"/>
-        <v>StunGun Gun</v>
+        <v>StunGun</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="9"/>
-        <v>StunGun Gun</v>
+        <f>C68</f>
+        <v>StunGun</v>
       </c>
       <c r="C68" s="94" t="s">
         <v>562</v>
@@ -42439,7 +42442,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="69" spans="1:25" hidden="1">
+    <row r="69" spans="1:25">
       <c r="A69" t="str">
         <f t="shared" si="7"/>
         <v>Wizard Staff</v>
@@ -42470,7 +42473,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="43" t="s">
-        <v>1812</v>
+        <v>3461</v>
       </c>
       <c r="K69" s="19"/>
       <c r="L69" s="19"/>
@@ -42492,7 +42495,7 @@
         <v>3448</v>
       </c>
     </row>
-    <row r="70" spans="1:25" hidden="1">
+    <row r="70" spans="1:25">
       <c r="A70" t="str">
         <f t="shared" si="7"/>
         <v>Sleep Book</v>
@@ -42545,7 +42548,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="71" spans="1:25" hidden="1">
+    <row r="71" spans="1:25">
       <c r="A71" t="str">
         <f t="shared" si="7"/>
         <v>Stone Book</v>
@@ -42598,7 +42601,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="72" spans="1:25" hidden="1">
+    <row r="72" spans="1:25">
       <c r="A72" t="str">
         <f t="shared" si="7"/>
         <v>Death Book</v>
@@ -48743,7 +48746,7 @@
         <v>3382</v>
       </c>
     </row>
-    <row r="196" spans="1:24">
+    <row r="196" spans="1:24" hidden="1">
       <c r="A196" t="str">
         <f t="shared" si="24"/>
         <v>Heart Magi</v>
@@ -49615,9 +49618,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Y213">
-    <filterColumn colId="18">
+    <filterColumn colId="15">
       <filters>
-        <filter val="Allies"/>
+        <filter val="Status"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Updated AGL weapons. Added char sheet printing
</commit_message>
<xml_diff>
--- a/FFL2 Data.xlsx
+++ b/FFL2 Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="150" yWindow="-225" windowWidth="28755" windowHeight="12540" activeTab="3"/>
+    <workbookView xWindow="150" yWindow="-225" windowWidth="28755" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11968" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11979" uniqueCount="2586">
   <si>
     <t>Monster</t>
   </si>
@@ -7801,6 +7801,24 @@
   </si>
   <si>
     <t>O-Dragon</t>
+  </si>
+  <si>
+    <t>Reduced multiplier from 11</t>
+  </si>
+  <si>
+    <t>Reduced multiplier by 13</t>
+  </si>
+  <si>
+    <t>Reduced multiplier by 9</t>
+  </si>
+  <si>
+    <t>Reduced multiplier from 7</t>
+  </si>
+  <si>
+    <t>Change to a Group or All attack?</t>
+  </si>
+  <si>
+    <t>Damage=Str*15; attack up to 7 times, depending on Agl vs mob;</t>
   </si>
 </sst>
 </file>
@@ -8584,7 +8602,22 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8891,9 +8924,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V252"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R248" sqref="R248"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24811,7 +24844,7 @@
         <v>2365</v>
       </c>
       <c r="C252">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G252" s="117">
         <v>1</v>
@@ -24837,8 +24870,16 @@
       <c r="O252" s="126" t="s">
         <v>441</v>
       </c>
+      <c r="P252" s="126" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A252">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -25396,6 +25437,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="18" t="s">
@@ -35025,16 +35070,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" filterMode="1"/>
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U231" sqref="U231"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="117"/>
@@ -35124,7 +35170,7 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="2" spans="1:27" hidden="1">
+    <row r="2" spans="1:27">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A65" si="0">B2</f>
         <v>Hammer</v>
@@ -35179,7 +35225,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1">
+    <row r="3" spans="1:27">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>Long Sword</v>
@@ -35236,7 +35282,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1">
+    <row r="4" spans="1:27">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Axe</v>
@@ -35293,7 +35339,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1">
+    <row r="5" spans="1:27">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Battle Sword</v>
@@ -35350,7 +35396,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1">
+    <row r="6" spans="1:27">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Katana</v>
@@ -35407,7 +35453,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1">
+    <row r="7" spans="1:27">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Gold Sword</v>
@@ -35464,7 +35510,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1">
+    <row r="8" spans="1:27">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Coral Sword</v>
@@ -35524,7 +35570,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1">
+    <row r="9" spans="1:27">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Ogre Axe</v>
@@ -35584,7 +35630,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1">
+    <row r="10" spans="1:27">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Dragon Sword</v>
@@ -35644,7 +35690,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1">
+    <row r="11" spans="1:27">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Sun Sword</v>
@@ -35704,7 +35750,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1">
+    <row r="12" spans="1:27">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Flame Sword</v>
@@ -35766,7 +35812,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1">
+    <row r="13" spans="1:27">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Ice Sword</v>
@@ -35828,7 +35874,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1">
+    <row r="14" spans="1:27">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Thunder Axe</v>
@@ -35890,7 +35936,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1">
+    <row r="15" spans="1:27">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Defend Sword</v>
@@ -35955,7 +36001,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1">
+    <row r="16" spans="1:27">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Rune Axe</v>
@@ -36018,7 +36064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:26" hidden="1">
+    <row r="17" spans="1:27">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Rapier</v>
@@ -36074,8 +36120,14 @@
       <c r="T17" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" hidden="1">
+      <c r="U17" t="s">
+        <v>2343</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>2583</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Gold Bow</v>
@@ -36142,7 +36194,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1">
+    <row r="19" spans="1:27">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Bronze Shield</v>
@@ -36196,7 +36248,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:26" hidden="1">
+    <row r="20" spans="1:27">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Silver Shield</v>
@@ -36250,7 +36302,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:26" hidden="1">
+    <row r="21" spans="1:27">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Gold Shield</v>
@@ -36304,7 +36356,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1">
+    <row r="22" spans="1:27">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Flame Shield</v>
@@ -36361,7 +36413,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:26" hidden="1">
+    <row r="23" spans="1:27">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Ice Shield</v>
@@ -36418,7 +36470,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1">
+    <row r="24" spans="1:27">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Dragon Shield</v>
@@ -36475,7 +36527,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1">
+    <row r="25" spans="1:27">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Cure Potion</v>
@@ -36532,7 +36584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1">
+    <row r="26" spans="1:27">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>X-Cure Potion</v>
@@ -36589,7 +36641,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:26" hidden="1">
+    <row r="27" spans="1:27">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Curse Potion</v>
@@ -36643,7 +36695,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="28" spans="1:26" hidden="1">
+    <row r="28" spans="1:27">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>EyeDrop</v>
@@ -36697,7 +36749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:26" hidden="1">
+    <row r="29" spans="1:27">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Abacus</v>
@@ -36752,7 +36804,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="30" spans="1:26" hidden="1">
+    <row r="30" spans="1:27">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Xcalibr Sword</v>
@@ -36817,7 +36869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:26" hidden="1">
+    <row r="31" spans="1:27">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Samurai Bow</v>
@@ -36881,7 +36933,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:26" hidden="1">
+    <row r="32" spans="1:27">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Cure Book</v>
@@ -36941,7 +36993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:25" hidden="1">
+    <row r="33" spans="1:25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Prayer Book</v>
@@ -37001,7 +37053,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="34" spans="1:25" hidden="1">
+    <row r="34" spans="1:25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Fire Book</v>
@@ -37061,7 +37113,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:25" hidden="1">
+    <row r="35" spans="1:25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Ice Book</v>
@@ -37121,7 +37173,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="36" spans="1:25" hidden="1">
+    <row r="36" spans="1:25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Thunder Book</v>
@@ -37181,7 +37233,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:25" hidden="1">
+    <row r="37" spans="1:25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Fog Book</v>
@@ -37241,7 +37293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:25" hidden="1">
+    <row r="38" spans="1:25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Sleep Book</v>
@@ -37298,7 +37350,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="39" spans="1:25" hidden="1">
+    <row r="39" spans="1:25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Stone Book</v>
@@ -37355,7 +37407,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="40" spans="1:25" hidden="1">
+    <row r="40" spans="1:25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Death Book</v>
@@ -37415,7 +37467,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="41" spans="1:25" hidden="1">
+    <row r="41" spans="1:25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Mage Staff</v>
@@ -37475,7 +37527,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:25" hidden="1">
+    <row r="42" spans="1:25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Wizard Staff</v>
@@ -37532,7 +37584,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="43" spans="1:25" hidden="1">
+    <row r="43" spans="1:25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Heal Staff</v>
@@ -37592,7 +37644,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:25" hidden="1">
+    <row r="44" spans="1:25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Flare Book</v>
@@ -37649,7 +37701,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="45" spans="1:25" hidden="1">
+    <row r="45" spans="1:25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Bronze Helm</v>
@@ -37693,7 +37745,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="46" spans="1:25" hidden="1">
+    <row r="46" spans="1:25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Silver Helm</v>
@@ -37737,7 +37789,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="47" spans="1:25" hidden="1">
+    <row r="47" spans="1:25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Gold Helm</v>
@@ -37781,7 +37833,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="48" spans="1:25" hidden="1">
+    <row r="48" spans="1:25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Dragon Helm</v>
@@ -37828,7 +37880,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="49" spans="1:25" hidden="1">
+    <row r="49" spans="1:25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Bronze Armor</v>
@@ -37872,7 +37924,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="50" spans="1:25" hidden="1">
+    <row r="50" spans="1:25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>Silver Armor</v>
@@ -37916,7 +37968,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="51" spans="1:25" hidden="1">
+    <row r="51" spans="1:25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Gold Armor</v>
@@ -37960,7 +38012,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="52" spans="1:25" hidden="1">
+    <row r="52" spans="1:25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Dragon Armor</v>
@@ -38007,7 +38059,7 @@
         <v>2387</v>
       </c>
     </row>
-    <row r="53" spans="1:25" hidden="1">
+    <row r="53" spans="1:25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Arthur Armor</v>
@@ -38054,7 +38106,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="54" spans="1:25" hidden="1">
+    <row r="54" spans="1:25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Bronze Glove</v>
@@ -38098,7 +38150,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="55" spans="1:25" hidden="1">
+    <row r="55" spans="1:25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Silver Glove</v>
@@ -38142,7 +38194,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="56" spans="1:25" hidden="1">
+    <row r="56" spans="1:25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Gold Glove</v>
@@ -38186,7 +38238,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="57" spans="1:25" hidden="1">
+    <row r="57" spans="1:25">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>Giant Glove</v>
@@ -38230,7 +38282,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="58" spans="1:25" hidden="1">
+    <row r="58" spans="1:25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Ninja Glove</v>
@@ -38277,7 +38329,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="59" spans="1:25" hidden="1">
+    <row r="59" spans="1:25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Hermes Boot</v>
@@ -38321,7 +38373,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="60" spans="1:25" hidden="1">
+    <row r="60" spans="1:25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Hecate Boot</v>
@@ -38365,7 +38417,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="61" spans="1:25" hidden="1">
+    <row r="61" spans="1:25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Elixier</v>
@@ -38417,7 +38469,7 @@
         <v>2576</v>
       </c>
     </row>
-    <row r="62" spans="1:25" hidden="1">
+    <row r="62" spans="1:25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Soft Potion</v>
@@ -38471,7 +38523,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="63" spans="1:25" hidden="1">
+    <row r="63" spans="1:25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Power Potion</v>
@@ -38515,7 +38567,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="64" spans="1:25" hidden="1">
+    <row r="64" spans="1:25">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Speed Potion</v>
@@ -38559,7 +38611,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="65" spans="1:27" hidden="1">
+    <row r="65" spans="1:27">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Magic Potion</v>
@@ -38603,7 +38655,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="66" spans="1:27" hidden="1">
+    <row r="66" spans="1:27">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A129" si="6">B66</f>
         <v>Body Potion</v>
@@ -38647,7 +38699,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="67" spans="1:27" hidden="1">
+    <row r="67" spans="1:27">
       <c r="A67" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">Tent </v>
@@ -38689,7 +38741,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="68" spans="1:27" hidden="1">
+    <row r="68" spans="1:27">
       <c r="A68" t="str">
         <f t="shared" si="6"/>
         <v>Whip</v>
@@ -38751,7 +38803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:27" hidden="1">
+    <row r="69" spans="1:27">
       <c r="A69" t="str">
         <f t="shared" si="6"/>
         <v>Blitz Whip</v>
@@ -38814,7 +38866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:27" hidden="1">
+    <row r="70" spans="1:27">
       <c r="A70" t="str">
         <f t="shared" si="6"/>
         <v>ChainSaw</v>
@@ -38869,7 +38921,7 @@
         <v>2397</v>
       </c>
     </row>
-    <row r="71" spans="1:27" hidden="1">
+    <row r="71" spans="1:27">
       <c r="A71" t="str">
         <f t="shared" si="6"/>
         <v>Counter</v>
@@ -38923,7 +38975,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:27" hidden="1">
+    <row r="72" spans="1:27">
       <c r="A72" t="str">
         <f t="shared" si="6"/>
         <v>Colt Gun</v>
@@ -38994,7 +39046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:27" hidden="1">
+    <row r="73" spans="1:27">
       <c r="A73" t="str">
         <f t="shared" si="6"/>
         <v>Musket Gun</v>
@@ -39063,7 +39115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:27" hidden="1">
+    <row r="74" spans="1:27">
       <c r="A74" t="str">
         <f t="shared" si="6"/>
         <v>Magnum Gun</v>
@@ -39132,7 +39184,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:27" hidden="1">
+    <row r="75" spans="1:27">
       <c r="A75" t="str">
         <f t="shared" si="6"/>
         <v>Chop Art</v>
@@ -39191,7 +39243,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="76" spans="1:27" hidden="1">
+    <row r="76" spans="1:27">
       <c r="A76" t="str">
         <f t="shared" si="6"/>
         <v>Kick Art</v>
@@ -39247,7 +39299,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="77" spans="1:27" hidden="1">
+    <row r="77" spans="1:27">
       <c r="A77" t="str">
         <f t="shared" si="6"/>
         <v>HeadBut Art</v>
@@ -39303,7 +39355,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="78" spans="1:27" hidden="1">
+    <row r="78" spans="1:27">
       <c r="A78" t="str">
         <f t="shared" si="6"/>
         <v>X-Kick Art</v>
@@ -39359,7 +39411,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="79" spans="1:27" hidden="1">
+    <row r="79" spans="1:27">
       <c r="A79" t="str">
         <f t="shared" si="6"/>
         <v>Jyudo Art</v>
@@ -39415,7 +39467,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="80" spans="1:27" hidden="1">
+    <row r="80" spans="1:27">
       <c r="A80" t="str">
         <f t="shared" si="6"/>
         <v>Karate Art</v>
@@ -39473,7 +39525,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="81" spans="1:26" hidden="1">
+    <row r="81" spans="1:26">
       <c r="A81" t="str">
         <f t="shared" si="6"/>
         <v>Temptat</v>
@@ -39528,7 +39580,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="82" spans="1:26" hidden="1">
+    <row r="82" spans="1:26">
       <c r="A82" t="str">
         <f t="shared" si="6"/>
         <v>StunGun</v>
@@ -39585,7 +39637,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="83" spans="1:26" hidden="1">
+    <row r="83" spans="1:26">
       <c r="A83" t="str">
         <f t="shared" si="6"/>
         <v>Heat</v>
@@ -39634,7 +39686,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="84" spans="1:26" hidden="1">
+    <row r="84" spans="1:26">
       <c r="A84" t="str">
         <f t="shared" si="6"/>
         <v>ComVirus</v>
@@ -39689,7 +39741,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="85" spans="1:26" hidden="1">
+    <row r="85" spans="1:26">
       <c r="A85" t="str">
         <f t="shared" si="6"/>
         <v>DNA</v>
@@ -39738,7 +39790,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="86" spans="1:26" hidden="1">
+    <row r="86" spans="1:26">
       <c r="A86" t="str">
         <f t="shared" si="6"/>
         <v>SMG Gun</v>
@@ -39803,7 +39855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:26" hidden="1">
+    <row r="87" spans="1:26">
       <c r="A87" t="str">
         <f t="shared" si="6"/>
         <v>Grenade</v>
@@ -39865,7 +39917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:26" hidden="1">
+    <row r="88" spans="1:26">
       <c r="A88" t="str">
         <f t="shared" si="6"/>
         <v>Bazooka Cannon</v>
@@ -39928,7 +39980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:26" hidden="1">
+    <row r="89" spans="1:26">
       <c r="A89" t="str">
         <f t="shared" si="6"/>
         <v>Vulcan Cannon</v>
@@ -39991,7 +40043,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:26" hidden="1">
+    <row r="90" spans="1:26">
       <c r="A90" t="str">
         <f t="shared" si="6"/>
         <v>Tank Cannon</v>
@@ -40060,7 +40112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:26" hidden="1">
+    <row r="91" spans="1:26">
       <c r="A91" t="str">
         <f t="shared" si="6"/>
         <v>Fire Gun</v>
@@ -40128,7 +40180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:26" hidden="1">
+    <row r="92" spans="1:26">
       <c r="A92" t="str">
         <f t="shared" si="6"/>
         <v>Missile Cannon</v>
@@ -40190,7 +40242,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:26" hidden="1">
+    <row r="93" spans="1:26">
       <c r="A93" t="str">
         <f t="shared" si="6"/>
         <v>NukeBomb</v>
@@ -40252,7 +40304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:26" hidden="1">
+    <row r="94" spans="1:26">
       <c r="A94" t="str">
         <f t="shared" si="6"/>
         <v>Giant Armor</v>
@@ -40296,7 +40348,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="95" spans="1:26" hidden="1">
+    <row r="95" spans="1:26">
       <c r="A95" t="str">
         <f t="shared" si="6"/>
         <v>Army Helm</v>
@@ -40340,7 +40392,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="96" spans="1:26" hidden="1">
+    <row r="96" spans="1:26">
       <c r="A96" t="str">
         <f t="shared" si="6"/>
         <v>Army Armor</v>
@@ -40384,7 +40436,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="97" spans="1:26" hidden="1">
+    <row r="97" spans="1:27">
       <c r="A97" t="str">
         <f t="shared" si="6"/>
         <v>Geta Boot</v>
@@ -40428,7 +40480,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="98" spans="1:26" hidden="1">
+    <row r="98" spans="1:27">
       <c r="A98" t="str">
         <f t="shared" si="6"/>
         <v>Sypha</v>
@@ -40483,7 +40535,7 @@
         <v>2308</v>
       </c>
     </row>
-    <row r="99" spans="1:26" hidden="1">
+    <row r="99" spans="1:27">
       <c r="A99" t="str">
         <f t="shared" si="6"/>
         <v>Coin</v>
@@ -40548,7 +40600,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:26" hidden="1">
+    <row r="100" spans="1:27">
       <c r="A100" t="str">
         <f t="shared" si="6"/>
         <v>Kimono Armor</v>
@@ -40592,7 +40644,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="101" spans="1:26" hidden="1">
+    <row r="101" spans="1:27">
       <c r="A101" t="str">
         <f t="shared" si="6"/>
         <v>Samurai Shield</v>
@@ -40646,7 +40698,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:26" hidden="1">
+    <row r="102" spans="1:27">
       <c r="A102" t="str">
         <f t="shared" si="6"/>
         <v>Muramas</v>
@@ -40706,7 +40758,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="103" spans="1:26" hidden="1">
+    <row r="103" spans="1:27">
       <c r="A103" t="str">
         <f t="shared" si="6"/>
         <v>Gungnir Spear</v>
@@ -40769,7 +40821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:26" hidden="1">
+    <row r="104" spans="1:27">
       <c r="A104" t="str">
         <f t="shared" si="6"/>
         <v>Laser Sword</v>
@@ -40825,8 +40877,14 @@
       <c r="T104" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="105" spans="1:26" hidden="1">
+      <c r="U104" t="s">
+        <v>2343</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27">
       <c r="A105" t="str">
         <f t="shared" si="6"/>
         <v>Psi Knife</v>
@@ -40883,7 +40941,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="106" spans="1:26" hidden="1">
+    <row r="106" spans="1:27">
       <c r="A106" t="str">
         <f t="shared" si="6"/>
         <v>Psi Sword</v>
@@ -40940,7 +40998,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="107" spans="1:26" hidden="1">
+    <row r="107" spans="1:27">
       <c r="A107" t="str">
         <f t="shared" si="6"/>
         <v>Laser Gun</v>
@@ -41000,7 +41058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:26" hidden="1">
+    <row r="108" spans="1:27">
       <c r="A108" t="str">
         <f t="shared" si="6"/>
         <v>SpeedUp</v>
@@ -41055,7 +41113,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="109" spans="1:26" hidden="1">
+    <row r="109" spans="1:27">
       <c r="A109" t="str">
         <f t="shared" si="6"/>
         <v>Rocket</v>
@@ -41120,7 +41178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="110" spans="1:26" hidden="1">
+    <row r="110" spans="1:27">
       <c r="A110" t="str">
         <f t="shared" si="6"/>
         <v>Psi Gun</v>
@@ -41177,7 +41235,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="111" spans="1:26" hidden="1">
+    <row r="111" spans="1:27">
       <c r="A111" t="str">
         <f t="shared" si="6"/>
         <v>Giant Helm</v>
@@ -41221,7 +41279,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="112" spans="1:26" hidden="1">
+    <row r="112" spans="1:27">
       <c r="A112" t="str">
         <f t="shared" si="6"/>
         <v>Hyper Cannon</v>
@@ -41277,7 +41335,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="113" spans="1:26" hidden="1">
+    <row r="113" spans="1:26">
       <c r="A113" t="str">
         <f t="shared" si="6"/>
         <v>Battle Armor</v>
@@ -41321,7 +41379,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="114" spans="1:26" hidden="1">
+    <row r="114" spans="1:26">
       <c r="A114" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">Parasuit </v>
@@ -41366,7 +41424,7 @@
         <v>2389</v>
       </c>
     </row>
-    <row r="115" spans="1:26" hidden="1">
+    <row r="115" spans="1:26">
       <c r="A115" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">Door </v>
@@ -41408,7 +41466,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="116" spans="1:26" hidden="1">
+    <row r="116" spans="1:26">
       <c r="A116" t="str">
         <f t="shared" si="6"/>
         <v>Micron Potion</v>
@@ -41452,7 +41510,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="117" spans="1:26" hidden="1">
+    <row r="117" spans="1:26">
       <c r="A117" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">Key </v>
@@ -41494,7 +41552,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="118" spans="1:26" hidden="1">
+    <row r="118" spans="1:26">
       <c r="A118" t="str">
         <f t="shared" si="6"/>
         <v>Masmune Magi</v>
@@ -41554,7 +41612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:26" hidden="1">
+    <row r="119" spans="1:26">
       <c r="A119" t="str">
         <f t="shared" si="6"/>
         <v>Aegis Magi</v>
@@ -41614,7 +41672,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:26" hidden="1">
+    <row r="120" spans="1:26">
       <c r="A120" t="str">
         <f t="shared" si="6"/>
         <v>Heart Magi</v>
@@ -41668,7 +41726,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="121" spans="1:26" hidden="1">
+    <row r="121" spans="1:26">
       <c r="A121" t="str">
         <f t="shared" si="6"/>
         <v>Pegasus Magi</v>
@@ -41713,7 +41771,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="122" spans="1:26" hidden="1">
+    <row r="122" spans="1:26">
       <c r="A122" t="str">
         <f t="shared" si="6"/>
         <v>Selfix</v>
@@ -41761,7 +41819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:26" hidden="1">
+    <row r="123" spans="1:26">
       <c r="A123" t="str">
         <f t="shared" si="6"/>
         <v>Seven Sword</v>
@@ -41796,7 +41854,7 @@
         <v>0</v>
       </c>
       <c r="K123" s="43" t="s">
-        <v>1992</v>
+        <v>2585</v>
       </c>
       <c r="L123" s="19"/>
       <c r="M123" s="19"/>
@@ -41812,13 +41870,16 @@
         <v>15</v>
       </c>
       <c r="S123" t="s">
-        <v>2350</v>
+        <v>2345</v>
       </c>
       <c r="T123" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="124" spans="1:26" hidden="1">
+      <c r="Y123" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="124" spans="1:26">
       <c r="A124" t="str">
         <f t="shared" si="6"/>
         <v>Nail</v>
@@ -41873,7 +41934,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="125" spans="1:26" hidden="1">
+    <row r="125" spans="1:26">
       <c r="A125" t="str">
         <f t="shared" si="6"/>
         <v>Tusk</v>
@@ -41928,7 +41989,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="126" spans="1:26" hidden="1">
+    <row r="126" spans="1:26">
       <c r="A126" t="str">
         <f t="shared" si="6"/>
         <v>Tongue</v>
@@ -41983,7 +42044,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="127" spans="1:26" hidden="1">
+    <row r="127" spans="1:26">
       <c r="A127" t="str">
         <f t="shared" si="6"/>
         <v>Stab</v>
@@ -42038,7 +42099,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="128" spans="1:26" hidden="1">
+    <row r="128" spans="1:26">
       <c r="A128" t="str">
         <f t="shared" si="6"/>
         <v>Branch</v>
@@ -42093,7 +42154,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="129" spans="1:25" hidden="1">
+    <row r="129" spans="1:27">
       <c r="A129" t="str">
         <f t="shared" si="6"/>
         <v>Bash</v>
@@ -42148,7 +42209,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="130" spans="1:25" hidden="1">
+    <row r="130" spans="1:27">
       <c r="A130" t="str">
         <f t="shared" ref="A130:A193" si="11">B130</f>
         <v>Punch</v>
@@ -42203,7 +42264,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="131" spans="1:25" hidden="1">
+    <row r="131" spans="1:27">
       <c r="A131" t="str">
         <f t="shared" si="11"/>
         <v>Kick</v>
@@ -42258,7 +42319,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="132" spans="1:25" hidden="1">
+    <row r="132" spans="1:27">
       <c r="A132" t="str">
         <f t="shared" si="11"/>
         <v>Horn</v>
@@ -42313,7 +42374,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="133" spans="1:25" hidden="1">
+    <row r="133" spans="1:27">
       <c r="A133" t="str">
         <f t="shared" si="11"/>
         <v>Thorn</v>
@@ -42368,7 +42429,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="134" spans="1:25" hidden="1">
+    <row r="134" spans="1:27">
       <c r="A134" t="str">
         <f t="shared" si="11"/>
         <v>Sword</v>
@@ -42423,7 +42484,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="135" spans="1:25" hidden="1">
+    <row r="135" spans="1:27">
       <c r="A135" t="str">
         <f t="shared" si="11"/>
         <v>Head</v>
@@ -42478,7 +42539,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="136" spans="1:25" hidden="1">
+    <row r="136" spans="1:27">
       <c r="A136" t="str">
         <f t="shared" si="11"/>
         <v>Beak</v>
@@ -42533,7 +42594,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="137" spans="1:25" hidden="1">
+    <row r="137" spans="1:27">
       <c r="A137" t="str">
         <f t="shared" si="11"/>
         <v>Tail</v>
@@ -42587,8 +42648,11 @@
       <c r="T137" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="138" spans="1:25" hidden="1">
+      <c r="AA137" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="138" spans="1:27">
       <c r="A138" t="str">
         <f t="shared" si="11"/>
         <v>Pincer</v>
@@ -42643,7 +42707,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="139" spans="1:25" hidden="1">
+    <row r="139" spans="1:27">
       <c r="A139" t="str">
         <f t="shared" si="11"/>
         <v>Fin</v>
@@ -42698,7 +42762,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="140" spans="1:25" hidden="1">
+    <row r="140" spans="1:27">
       <c r="A140" t="str">
         <f t="shared" si="11"/>
         <v>Tentacle</v>
@@ -42753,7 +42817,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="141" spans="1:25" hidden="1">
+    <row r="141" spans="1:27">
       <c r="A141" t="str">
         <f t="shared" si="11"/>
         <v>W-Pincer</v>
@@ -42809,7 +42873,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="142" spans="1:25" hidden="1">
+    <row r="142" spans="1:27">
       <c r="A142" t="str">
         <f t="shared" si="11"/>
         <v>W-Attack</v>
@@ -42867,7 +42931,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="143" spans="1:25" hidden="1">
+    <row r="143" spans="1:27">
       <c r="A143" t="str">
         <f t="shared" si="11"/>
         <v>4-Heads</v>
@@ -42925,7 +42989,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="144" spans="1:25" hidden="1">
+    <row r="144" spans="1:27">
       <c r="A144" t="str">
         <f t="shared" si="11"/>
         <v>8-Legs</v>
@@ -42983,7 +43047,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="145" spans="1:27" hidden="1">
+    <row r="145" spans="1:27">
       <c r="A145" t="str">
         <f t="shared" si="11"/>
         <v>Touch</v>
@@ -43042,7 +43106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="1:27" hidden="1">
+    <row r="146" spans="1:27">
       <c r="A146" t="str">
         <f t="shared" si="11"/>
         <v>Saw</v>
@@ -43095,7 +43159,7 @@
         <v>2397</v>
       </c>
     </row>
-    <row r="147" spans="1:27" hidden="1">
+    <row r="147" spans="1:27">
       <c r="A147" t="str">
         <f t="shared" si="11"/>
         <v>Dissolve</v>
@@ -43154,7 +43218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="148" spans="1:27" hidden="1">
+    <row r="148" spans="1:27">
       <c r="A148" t="str">
         <f t="shared" si="11"/>
         <v>Absorb</v>
@@ -43213,7 +43277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="149" spans="1:27" hidden="1">
+    <row r="149" spans="1:27">
       <c r="A149" t="str">
         <f t="shared" si="11"/>
         <v>Cure</v>
@@ -43269,7 +43333,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="150" spans="1:27" hidden="1">
+    <row r="150" spans="1:27">
       <c r="A150" t="str">
         <f t="shared" si="11"/>
         <v>Defense</v>
@@ -43319,7 +43383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="151" spans="1:27" hidden="1">
+    <row r="151" spans="1:27">
       <c r="A151" t="str">
         <f t="shared" si="11"/>
         <v>Shell</v>
@@ -43369,7 +43433,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:27" hidden="1">
+    <row r="152" spans="1:27">
       <c r="A152" t="str">
         <f t="shared" si="11"/>
         <v>Mirror</v>
@@ -43416,7 +43480,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="153" spans="1:27" hidden="1">
+    <row r="153" spans="1:27">
       <c r="A153" t="str">
         <f t="shared" si="11"/>
         <v>Backlash</v>
@@ -43469,7 +43533,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="154" spans="1:27" hidden="1">
+    <row r="154" spans="1:27">
       <c r="A154" t="str">
         <f t="shared" si="11"/>
         <v>Burning</v>
@@ -43525,7 +43589,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="155" spans="1:27" hidden="1">
+    <row r="155" spans="1:27">
       <c r="A155" t="str">
         <f t="shared" si="11"/>
         <v>2-Swords</v>
@@ -43581,7 +43645,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="156" spans="1:27" hidden="1">
+    <row r="156" spans="1:27">
       <c r="A156" t="str">
         <f t="shared" si="11"/>
         <v>2-Tusks</v>
@@ -43637,7 +43701,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="157" spans="1:27" hidden="1">
+    <row r="157" spans="1:27">
       <c r="A157" t="str">
         <f t="shared" si="11"/>
         <v>3-Heads</v>
@@ -43695,7 +43759,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="158" spans="1:27" hidden="1">
+    <row r="158" spans="1:27">
       <c r="A158" t="str">
         <f t="shared" si="11"/>
         <v>3-Horns</v>
@@ -43753,7 +43817,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="159" spans="1:27" hidden="1">
+    <row r="159" spans="1:27">
       <c r="A159" t="str">
         <f t="shared" si="11"/>
         <v>6-Arms</v>
@@ -43809,7 +43873,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="160" spans="1:27" hidden="1">
+    <row r="160" spans="1:27">
       <c r="A160" t="str">
         <f t="shared" si="11"/>
         <v>Critical</v>
@@ -43865,7 +43929,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="161" spans="1:27" hidden="1">
+    <row r="161" spans="1:27">
       <c r="A161" t="str">
         <f t="shared" si="11"/>
         <v>Axe</v>
@@ -43920,7 +43984,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="162" spans="1:27" hidden="1">
+    <row r="162" spans="1:27">
       <c r="A162" t="str">
         <f t="shared" si="11"/>
         <v>Honey</v>
@@ -43976,7 +44040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:27" hidden="1">
+    <row r="163" spans="1:27">
       <c r="A163" t="str">
         <f t="shared" si="11"/>
         <v>Heal</v>
@@ -44032,7 +44096,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="164" spans="1:27" hidden="1">
+    <row r="164" spans="1:27">
       <c r="A164" t="str">
         <f t="shared" si="11"/>
         <v>MegaCure</v>
@@ -44092,7 +44156,7 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="165" spans="1:27" hidden="1">
+    <row r="165" spans="1:27">
       <c r="A165" t="str">
         <f t="shared" si="11"/>
         <v>W-Kick</v>
@@ -44148,7 +44212,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="166" spans="1:27" hidden="1">
+    <row r="166" spans="1:27">
       <c r="A166" t="str">
         <f t="shared" si="11"/>
         <v>ParaNail</v>
@@ -44201,7 +44265,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="167" spans="1:27" hidden="1">
+    <row r="167" spans="1:27">
       <c r="A167" t="str">
         <f t="shared" si="11"/>
         <v>Wind Up</v>
@@ -44254,7 +44318,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="168" spans="1:27" hidden="1">
+    <row r="168" spans="1:27">
       <c r="A168" t="str">
         <f t="shared" si="11"/>
         <v>Tie Up</v>
@@ -44307,7 +44371,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="169" spans="1:27" hidden="1">
+    <row r="169" spans="1:27">
       <c r="A169" t="str">
         <f t="shared" si="11"/>
         <v>Breath</v>
@@ -44360,7 +44424,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="170" spans="1:27" hidden="1">
+    <row r="170" spans="1:27">
       <c r="A170" t="str">
         <f t="shared" si="11"/>
         <v>Poison</v>
@@ -44413,7 +44477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:27" hidden="1">
+    <row r="171" spans="1:27">
       <c r="A171" t="str">
         <f t="shared" si="11"/>
         <v>P-Skin</v>
@@ -44466,7 +44530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:27" hidden="1">
+    <row r="172" spans="1:27">
       <c r="A172" t="str">
         <f t="shared" si="11"/>
         <v>ParaSkin</v>
@@ -44519,7 +44583,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="173" spans="1:27" hidden="1">
+    <row r="173" spans="1:27">
       <c r="A173" t="str">
         <f t="shared" si="11"/>
         <v>Petrify</v>
@@ -44572,7 +44636,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="174" spans="1:27" hidden="1">
+    <row r="174" spans="1:27">
       <c r="A174" t="str">
         <f t="shared" si="11"/>
         <v>StonSkin</v>
@@ -44625,7 +44689,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="175" spans="1:27" hidden="1">
+    <row r="175" spans="1:27">
       <c r="A175" t="str">
         <f t="shared" si="11"/>
         <v>Thunder</v>
@@ -44681,7 +44745,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="176" spans="1:27" hidden="1">
+    <row r="176" spans="1:27">
       <c r="A176" t="str">
         <f t="shared" si="11"/>
         <v>Ice</v>
@@ -44737,7 +44801,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="177" spans="1:24" hidden="1">
+    <row r="177" spans="1:24">
       <c r="A177" t="str">
         <f t="shared" si="11"/>
         <v>Fire</v>
@@ -44793,7 +44857,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="178" spans="1:24" hidden="1">
+    <row r="178" spans="1:24">
       <c r="A178" t="str">
         <f t="shared" si="11"/>
         <v>Flame</v>
@@ -44849,7 +44913,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="179" spans="1:24" hidden="1">
+    <row r="179" spans="1:24">
       <c r="A179" t="str">
         <f t="shared" si="11"/>
         <v>Gas</v>
@@ -44905,7 +44969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="180" spans="1:24" hidden="1">
+    <row r="180" spans="1:24">
       <c r="A180" t="str">
         <f t="shared" si="11"/>
         <v>Blizzard</v>
@@ -44961,7 +45025,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="181" spans="1:24" hidden="1">
+    <row r="181" spans="1:24">
       <c r="A181" t="str">
         <f t="shared" si="11"/>
         <v>Lightning</v>
@@ -45017,7 +45081,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="182" spans="1:24" hidden="1">
+    <row r="182" spans="1:24">
       <c r="A182" t="str">
         <f t="shared" si="11"/>
         <v>Beam</v>
@@ -45070,7 +45134,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="183" spans="1:24" hidden="1">
+    <row r="183" spans="1:24">
       <c r="A183" t="str">
         <f t="shared" si="11"/>
         <v>P-Blast</v>
@@ -45123,7 +45187,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="184" spans="1:24" hidden="1">
+    <row r="184" spans="1:24">
       <c r="A184" t="str">
         <f t="shared" si="11"/>
         <v>Dispel</v>
@@ -45179,7 +45243,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="185" spans="1:24" hidden="1">
+    <row r="185" spans="1:24">
       <c r="A185" t="str">
         <f t="shared" si="11"/>
         <v>D-Beam</v>
@@ -45235,7 +45299,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="186" spans="1:24" hidden="1">
+    <row r="186" spans="1:24">
       <c r="A186" t="str">
         <f t="shared" si="11"/>
         <v>Squirt</v>
@@ -45291,7 +45355,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="187" spans="1:24" hidden="1">
+    <row r="187" spans="1:24">
       <c r="A187" t="str">
         <f t="shared" si="11"/>
         <v>SunBurst</v>
@@ -45347,7 +45411,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="188" spans="1:24" hidden="1">
+    <row r="188" spans="1:24">
       <c r="A188" t="str">
         <f t="shared" si="11"/>
         <v>SleepGas</v>
@@ -45400,7 +45464,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="189" spans="1:24" hidden="1">
+    <row r="189" spans="1:24">
       <c r="A189" t="str">
         <f t="shared" si="11"/>
         <v>Sleep</v>
@@ -45453,7 +45517,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="190" spans="1:24" hidden="1">
+    <row r="190" spans="1:24">
       <c r="A190" t="str">
         <f t="shared" si="11"/>
         <v>StonGaze</v>
@@ -45506,7 +45570,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="191" spans="1:24" hidden="1">
+    <row r="191" spans="1:24">
       <c r="A191" t="str">
         <f t="shared" si="11"/>
         <v>Stone</v>
@@ -45559,7 +45623,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="192" spans="1:24" hidden="1">
+    <row r="192" spans="1:24">
       <c r="A192" t="str">
         <f t="shared" si="11"/>
         <v>StoneGas</v>
@@ -45612,7 +45676,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="193" spans="1:25" hidden="1">
+    <row r="193" spans="1:25">
       <c r="A193" t="str">
         <f t="shared" si="11"/>
         <v>FatalGas</v>
@@ -45665,7 +45729,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="194" spans="1:25" hidden="1">
+    <row r="194" spans="1:25">
       <c r="A194" t="str">
         <f t="shared" ref="A194:A258" si="14">B194</f>
         <v>X-Gaze</v>
@@ -45718,7 +45782,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="195" spans="1:25" hidden="1">
+    <row r="195" spans="1:25">
       <c r="A195" t="str">
         <f t="shared" si="14"/>
         <v>Erase</v>
@@ -45771,7 +45835,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="196" spans="1:25" hidden="1">
+    <row r="196" spans="1:25">
       <c r="A196" t="str">
         <f t="shared" si="14"/>
         <v>Blind</v>
@@ -45824,7 +45888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:25" hidden="1">
+    <row r="197" spans="1:25">
       <c r="A197" t="str">
         <f t="shared" si="14"/>
         <v>Flash</v>
@@ -45877,7 +45941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="198" spans="1:25" hidden="1">
+    <row r="198" spans="1:25">
       <c r="A198" t="str">
         <f t="shared" si="14"/>
         <v>Ink</v>
@@ -45930,7 +45994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="199" spans="1:25" hidden="1">
+    <row r="199" spans="1:25">
       <c r="A199" t="str">
         <f t="shared" si="14"/>
         <v>PoisonCloud</v>
@@ -45983,7 +46047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:25" hidden="1">
+    <row r="200" spans="1:25">
       <c r="A200" t="str">
         <f t="shared" si="14"/>
         <v>Gaze</v>
@@ -46036,7 +46100,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="201" spans="1:25" hidden="1">
+    <row r="201" spans="1:25">
       <c r="A201" t="str">
         <f t="shared" si="14"/>
         <v>Stunner</v>
@@ -46089,7 +46153,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="202" spans="1:25" hidden="1">
+    <row r="202" spans="1:25">
       <c r="A202" t="str">
         <f t="shared" si="14"/>
         <v>Gaze</v>
@@ -46142,7 +46206,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="203" spans="1:25" hidden="1">
+    <row r="203" spans="1:25">
       <c r="A203" t="str">
         <f t="shared" si="14"/>
         <v>Charm</v>
@@ -46195,7 +46259,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="204" spans="1:25" hidden="1">
+    <row r="204" spans="1:25">
       <c r="A204" t="str">
         <f t="shared" si="14"/>
         <v>Hypnos</v>
@@ -46248,7 +46312,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="205" spans="1:25" hidden="1">
+    <row r="205" spans="1:25">
       <c r="A205" t="str">
         <f t="shared" si="14"/>
         <v>Sand</v>
@@ -46301,7 +46365,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="206" spans="1:25" hidden="1">
+    <row r="206" spans="1:25">
       <c r="A206" t="str">
         <f t="shared" si="14"/>
         <v>Cobweb</v>
@@ -46354,7 +46418,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="207" spans="1:25" hidden="1">
+    <row r="207" spans="1:25">
       <c r="A207" t="str">
         <f t="shared" si="14"/>
         <v>Blitz</v>
@@ -46407,7 +46471,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="208" spans="1:25" hidden="1">
+    <row r="208" spans="1:25">
       <c r="A208" t="str">
         <f t="shared" si="14"/>
         <v>Drain</v>
@@ -46460,7 +46524,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="209" spans="1:25" hidden="1">
+    <row r="209" spans="1:25">
       <c r="A209" t="str">
         <f t="shared" si="14"/>
         <v>Stench</v>
@@ -46513,7 +46577,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="210" spans="1:25" hidden="1">
+    <row r="210" spans="1:25">
       <c r="A210" t="str">
         <f t="shared" si="14"/>
         <v>Haste</v>
@@ -46566,7 +46630,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="211" spans="1:25" hidden="1">
+    <row r="211" spans="1:25">
       <c r="A211" t="str">
         <f t="shared" si="14"/>
         <v>Tornado</v>
@@ -46619,7 +46683,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="212" spans="1:25" hidden="1">
+    <row r="212" spans="1:25">
       <c r="A212" t="str">
         <f t="shared" si="14"/>
         <v>Quake</v>
@@ -46675,7 +46739,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="213" spans="1:25" hidden="1">
+    <row r="213" spans="1:25">
       <c r="A213" t="str">
         <f t="shared" si="14"/>
         <v>Whirl</v>
@@ -46728,7 +46792,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="214" spans="1:25" hidden="1">
+    <row r="214" spans="1:25">
       <c r="A214" t="str">
         <f t="shared" si="14"/>
         <v>Flare</v>
@@ -46781,7 +46845,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="215" spans="1:25" hidden="1">
+    <row r="215" spans="1:25">
       <c r="A215" t="str">
         <f t="shared" si="14"/>
         <v>Steal</v>
@@ -46834,7 +46898,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="216" spans="1:25" hidden="1">
+    <row r="216" spans="1:25">
       <c r="A216" t="str">
         <f t="shared" si="14"/>
         <v>Explode</v>
@@ -46890,7 +46954,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="217" spans="1:25" hidden="1">
+    <row r="217" spans="1:25">
       <c r="A217" t="str">
         <f t="shared" si="14"/>
         <v>Acid</v>
@@ -46946,7 +47010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="218" spans="1:25" hidden="1">
+    <row r="218" spans="1:25">
       <c r="A218" t="str">
         <f t="shared" si="14"/>
         <v>Riddle</v>
@@ -46999,7 +47063,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="219" spans="1:25" hidden="1">
+    <row r="219" spans="1:25">
       <c r="A219" t="str">
         <f t="shared" si="14"/>
         <v>CursSong</v>
@@ -47052,7 +47116,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="220" spans="1:25" hidden="1">
+    <row r="220" spans="1:25">
       <c r="A220" t="str">
         <f t="shared" si="14"/>
         <v>MadSong</v>
@@ -47193,7 +47257,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="223" spans="1:25" hidden="1">
+    <row r="223" spans="1:25">
       <c r="A223" t="str">
         <f t="shared" si="14"/>
         <v>Multiply</v>
@@ -47886,7 +47950,7 @@
         <v>2394</v>
       </c>
     </row>
-    <row r="237" spans="1:27" hidden="1">
+    <row r="237" spans="1:27">
       <c r="A237" t="str">
         <f t="shared" si="14"/>
         <v>Teleport</v>
@@ -47926,7 +47990,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="238" spans="1:27" hidden="1">
+    <row r="238" spans="1:27">
       <c r="A238" t="str">
         <f t="shared" si="14"/>
         <v>Remedy</v>
@@ -48022,7 +48086,7 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="240" spans="1:27" hidden="1">
+    <row r="240" spans="1:27">
       <c r="A240" t="str">
         <f t="shared" si="14"/>
         <v>PoisonBurst</v>
@@ -48078,7 +48142,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="241" spans="1:26" hidden="1">
+    <row r="241" spans="1:27">
       <c r="A241" t="str">
         <f t="shared" si="14"/>
         <v>FlareApollo</v>
@@ -48124,7 +48188,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="242" spans="1:26" hidden="1">
+    <row r="242" spans="1:27">
       <c r="A242" t="str">
         <f t="shared" si="14"/>
         <v>Smasher</v>
@@ -48168,7 +48232,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="243" spans="1:26">
+    <row r="243" spans="1:27">
       <c r="A243" t="str">
         <f t="shared" si="14"/>
         <v>Recover</v>
@@ -48208,7 +48272,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="244" spans="1:26" hidden="1">
+    <row r="244" spans="1:27">
       <c r="A244" t="str">
         <f t="shared" si="14"/>
         <v>Power Magi</v>
@@ -48253,7 +48317,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="245" spans="1:26" hidden="1">
+    <row r="245" spans="1:27">
       <c r="A245" t="str">
         <f t="shared" si="14"/>
         <v>Speed Magi</v>
@@ -48298,7 +48362,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="246" spans="1:26" hidden="1">
+    <row r="246" spans="1:27">
       <c r="A246" t="str">
         <f t="shared" si="14"/>
         <v>Mana Magi</v>
@@ -48343,7 +48407,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="247" spans="1:26" hidden="1">
+    <row r="247" spans="1:27">
       <c r="A247" t="str">
         <f t="shared" si="14"/>
         <v>Defense Magi</v>
@@ -48388,7 +48452,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="248" spans="1:26" hidden="1">
+    <row r="248" spans="1:27">
       <c r="A248" t="str">
         <f t="shared" si="14"/>
         <v>Fire Magi</v>
@@ -48436,7 +48500,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="249" spans="1:26" hidden="1">
+    <row r="249" spans="1:27">
       <c r="A249" t="str">
         <f t="shared" si="14"/>
         <v>Ice Magi</v>
@@ -48484,7 +48548,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="250" spans="1:26" hidden="1">
+    <row r="250" spans="1:27">
       <c r="A250" t="str">
         <f t="shared" si="14"/>
         <v>Thunder Magi</v>
@@ -48532,7 +48596,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="251" spans="1:26" hidden="1">
+    <row r="251" spans="1:27">
       <c r="A251" t="str">
         <f t="shared" si="14"/>
         <v>Poison Magi</v>
@@ -48580,7 +48644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="252" spans="1:26" hidden="1">
+    <row r="252" spans="1:27">
       <c r="A252" t="str">
         <f t="shared" si="14"/>
         <v>CatClaw</v>
@@ -48636,8 +48700,14 @@
       <c r="T252" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="253" spans="1:26" hidden="1">
+      <c r="U252" t="s">
+        <v>2343</v>
+      </c>
+      <c r="AA252" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="253" spans="1:27">
       <c r="A253" t="str">
         <f t="shared" si="14"/>
         <v>Vampic Sword</v>
@@ -48700,7 +48770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="254" spans="1:26" hidden="1">
+    <row r="254" spans="1:27">
       <c r="A254" t="str">
         <f t="shared" si="14"/>
         <v>Glass Sword</v>
@@ -48765,7 +48835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="255" spans="1:26" hidden="1">
+    <row r="255" spans="1:27">
       <c r="A255" t="str">
         <f t="shared" si="14"/>
         <v>Revenge Sword</v>
@@ -48819,7 +48889,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="256" spans="1:26" hidden="1">
+    <row r="256" spans="1:27">
       <c r="A256" t="str">
         <f t="shared" si="14"/>
         <v>Bow</v>
@@ -48886,7 +48956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="257" spans="1:27" hidden="1">
+    <row r="257" spans="1:27">
       <c r="A257" t="str">
         <f t="shared" si="14"/>
         <v>Sabre</v>
@@ -48942,6 +49012,12 @@
       <c r="T257" t="s">
         <v>2307</v>
       </c>
+      <c r="U257" t="s">
+        <v>2343</v>
+      </c>
+      <c r="AA257" t="s">
+        <v>2582</v>
+      </c>
     </row>
     <row r="258" spans="1:27">
       <c r="A258" t="str">
@@ -48973,11 +49049,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AA258">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="Trait"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:AA257">
       <sortCondition ref="E1:E257"/>
     </sortState>
@@ -48988,8 +49059,13 @@
     <sortCondition ref="T2:T213"/>
     <sortCondition ref="F2:F213"/>
   </sortState>
+  <conditionalFormatting sqref="A2:A258">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Rewrote Group and All Enemies. Added removeCondition
</commit_message>
<xml_diff>
--- a/FFL2 Data.xlsx
+++ b/FFL2 Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Action IV\Documents\GitHub\pillar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52B6599-561A-42A3-AE40-73C63B64A8F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C4839F-ECCF-4930-BC14-D52FD04C5FE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12237" uniqueCount="2606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12237" uniqueCount="2604">
   <si>
     <t>Monster</t>
   </si>
@@ -7177,9 +7177,6 @@
     <t>Stun</t>
   </si>
   <si>
-    <t>Holy</t>
-  </si>
-  <si>
     <t>Debuff</t>
   </si>
   <si>
@@ -7814,9 +7811,6 @@
   </si>
   <si>
     <t>Damage=Str*15; attack up to 7 times, depending on Agl vs mob;</t>
-  </si>
-  <si>
-    <t>Accurate</t>
   </si>
   <si>
     <t>Family</t>
@@ -9023,8 +9017,8 @@
   <dimension ref="A1:W253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O172" sqref="O172"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9108,7 +9102,7 @@
         <v>2328</v>
       </c>
       <c r="W1" s="140" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -10110,7 +10104,7 @@
       <c r="U16" s="6"/>
       <c r="V16" s="7"/>
       <c r="W16" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -10172,7 +10166,7 @@
       <c r="U17" s="6"/>
       <c r="V17" s="7"/>
       <c r="W17" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -10238,7 +10232,7 @@
       <c r="U18" s="6"/>
       <c r="V18" s="7"/>
       <c r="W18" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -10308,7 +10302,7 @@
       </c>
       <c r="V19" s="7"/>
       <c r="W19" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -10380,7 +10374,7 @@
         <v>70</v>
       </c>
       <c r="W20" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -10440,7 +10434,7 @@
       <c r="U21" s="6"/>
       <c r="V21" s="7"/>
       <c r="W21" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -10504,7 +10498,7 @@
       <c r="U22" s="6"/>
       <c r="V22" s="7"/>
       <c r="W22" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -10570,7 +10564,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="7"/>
       <c r="W23" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -10640,7 +10634,7 @@
       </c>
       <c r="V24" s="7"/>
       <c r="W24" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -10712,7 +10706,7 @@
         <v>70</v>
       </c>
       <c r="W25" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -10774,7 +10768,7 @@
       <c r="U26" s="6"/>
       <c r="V26" s="7"/>
       <c r="W26" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -10840,7 +10834,7 @@
       <c r="U27" s="6"/>
       <c r="V27" s="7"/>
       <c r="W27" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -10908,7 +10902,7 @@
       <c r="U28" s="6"/>
       <c r="V28" s="7"/>
       <c r="W28" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -10978,7 +10972,7 @@
       </c>
       <c r="V29" s="7"/>
       <c r="W29" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -11050,7 +11044,7 @@
         <v>70</v>
       </c>
       <c r="W30" s="134" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -11110,7 +11104,7 @@
       <c r="U31" s="6"/>
       <c r="V31" s="7"/>
       <c r="W31" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -11172,7 +11166,7 @@
       <c r="U32" s="6"/>
       <c r="V32" s="7"/>
       <c r="W32" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -11238,7 +11232,7 @@
       <c r="U33" s="6"/>
       <c r="V33" s="7"/>
       <c r="W33" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="34" spans="1:23">
@@ -11308,7 +11302,7 @@
       </c>
       <c r="V34" s="7"/>
       <c r="W34" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="35" spans="1:23">
@@ -11380,7 +11374,7 @@
         <v>139</v>
       </c>
       <c r="W35" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -11440,7 +11434,7 @@
       <c r="U36" s="6"/>
       <c r="V36" s="7"/>
       <c r="W36" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="37" spans="1:23">
@@ -11504,7 +11498,7 @@
       <c r="U37" s="6"/>
       <c r="V37" s="7"/>
       <c r="W37" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -11572,7 +11566,7 @@
       <c r="U38" s="6"/>
       <c r="V38" s="7"/>
       <c r="W38" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -11642,7 +11636,7 @@
       </c>
       <c r="V39" s="7"/>
       <c r="W39" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -11714,7 +11708,7 @@
         <v>50</v>
       </c>
       <c r="W40" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="41" spans="1:23">
@@ -11776,7 +11770,7 @@
       <c r="U41" s="6"/>
       <c r="V41" s="7"/>
       <c r="W41" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="42" spans="1:23">
@@ -11842,7 +11836,7 @@
       <c r="U42" s="6"/>
       <c r="V42" s="7"/>
       <c r="W42" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="43" spans="1:23">
@@ -11910,7 +11904,7 @@
       <c r="U43" s="6"/>
       <c r="V43" s="7"/>
       <c r="W43" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="44" spans="1:23">
@@ -11967,7 +11961,7 @@
         <v>165</v>
       </c>
       <c r="R44" s="6" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="S44" s="6" t="s">
         <v>173</v>
@@ -11980,7 +11974,7 @@
       </c>
       <c r="V44" s="7"/>
       <c r="W44" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -12040,7 +12034,7 @@
         <v>173</v>
       </c>
       <c r="S45" s="9" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="T45" s="9" t="s">
         <v>69</v>
@@ -12052,7 +12046,7 @@
         <v>139</v>
       </c>
       <c r="W45" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -13112,7 +13106,7 @@
       <c r="U61" s="6"/>
       <c r="V61" s="7"/>
       <c r="W61" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="62" spans="1:23">
@@ -13174,7 +13168,7 @@
       <c r="U62" s="6"/>
       <c r="V62" s="7"/>
       <c r="W62" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="63" spans="1:23">
@@ -13242,7 +13236,7 @@
       <c r="U63" s="6"/>
       <c r="V63" s="7"/>
       <c r="W63" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="64" spans="1:23">
@@ -13312,7 +13306,7 @@
       </c>
       <c r="V64" s="7"/>
       <c r="W64" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="65" spans="1:23">
@@ -13384,7 +13378,7 @@
         <v>50</v>
       </c>
       <c r="W65" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="66" spans="1:23">
@@ -13444,7 +13438,7 @@
       <c r="U66" s="6"/>
       <c r="V66" s="7"/>
       <c r="W66" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="67" spans="1:23">
@@ -13510,7 +13504,7 @@
       <c r="U67" s="6"/>
       <c r="V67" s="7"/>
       <c r="W67" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="68" spans="1:23">
@@ -13578,7 +13572,7 @@
       <c r="U68" s="6"/>
       <c r="V68" s="7"/>
       <c r="W68" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="69" spans="1:23">
@@ -13648,7 +13642,7 @@
       </c>
       <c r="V69" s="7"/>
       <c r="W69" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="70" spans="1:23">
@@ -13720,7 +13714,7 @@
         <v>50</v>
       </c>
       <c r="W70" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="71" spans="1:23">
@@ -13780,7 +13774,7 @@
       <c r="U71" s="6"/>
       <c r="V71" s="7"/>
       <c r="W71" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="72" spans="1:23">
@@ -13846,7 +13840,7 @@
       <c r="U72" s="6"/>
       <c r="V72" s="7"/>
       <c r="W72" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="73" spans="1:23">
@@ -13914,7 +13908,7 @@
       <c r="U73" s="6"/>
       <c r="V73" s="7"/>
       <c r="W73" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="74" spans="1:23">
@@ -13984,7 +13978,7 @@
       </c>
       <c r="V74" s="7"/>
       <c r="W74" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="75" spans="1:23">
@@ -14056,7 +14050,7 @@
         <v>50</v>
       </c>
       <c r="W75" s="134" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="76" spans="1:23">
@@ -15122,7 +15116,7 @@
       <c r="U91" s="6"/>
       <c r="V91" s="7"/>
       <c r="W91" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="92" spans="1:23">
@@ -15184,7 +15178,7 @@
       <c r="U92" s="6"/>
       <c r="V92" s="7"/>
       <c r="W92" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="93" spans="1:23">
@@ -15250,7 +15244,7 @@
       <c r="U93" s="6"/>
       <c r="V93" s="7"/>
       <c r="W93" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="94" spans="1:23">
@@ -15320,7 +15314,7 @@
       </c>
       <c r="V94" s="7"/>
       <c r="W94" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -15392,7 +15386,7 @@
         <v>70</v>
       </c>
       <c r="W95" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="96" spans="1:23">
@@ -15452,7 +15446,7 @@
       <c r="U96" s="6"/>
       <c r="V96" s="7"/>
       <c r="W96" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="97" spans="1:23">
@@ -15518,7 +15512,7 @@
       <c r="U97" s="6"/>
       <c r="V97" s="7"/>
       <c r="W97" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="98" spans="1:23">
@@ -15586,7 +15580,7 @@
       <c r="U98" s="6"/>
       <c r="V98" s="7"/>
       <c r="W98" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="99" spans="1:23">
@@ -15656,7 +15650,7 @@
       </c>
       <c r="V99" s="7"/>
       <c r="W99" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="100" spans="1:23">
@@ -15728,7 +15722,7 @@
         <v>214</v>
       </c>
       <c r="W100" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="101" spans="1:23">
@@ -15792,7 +15786,7 @@
       <c r="U101" s="6"/>
       <c r="V101" s="7"/>
       <c r="W101" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="102" spans="1:23">
@@ -15858,7 +15852,7 @@
       <c r="U102" s="6"/>
       <c r="V102" s="7"/>
       <c r="W102" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="103" spans="1:23">
@@ -15926,7 +15920,7 @@
       <c r="U103" s="6"/>
       <c r="V103" s="7"/>
       <c r="W103" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="104" spans="1:23">
@@ -15996,7 +15990,7 @@
       </c>
       <c r="V104" s="7"/>
       <c r="W104" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="105" spans="1:23">
@@ -16053,7 +16047,7 @@
         <v>150</v>
       </c>
       <c r="R105" s="9" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="S105" s="9" t="s">
         <v>101</v>
@@ -16068,7 +16062,7 @@
         <v>105</v>
       </c>
       <c r="W105" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="106" spans="1:23">
@@ -16128,7 +16122,7 @@
       <c r="U106" s="6"/>
       <c r="V106" s="7"/>
       <c r="W106" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="107" spans="1:23">
@@ -16190,7 +16184,7 @@
       <c r="U107" s="6"/>
       <c r="V107" s="7"/>
       <c r="W107" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="108" spans="1:23">
@@ -16256,7 +16250,7 @@
       <c r="U108" s="6"/>
       <c r="V108" s="7"/>
       <c r="W108" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="109" spans="1:23">
@@ -16319,14 +16313,14 @@
         <v>25</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="U109" s="6" t="s">
         <v>139</v>
       </c>
       <c r="V109" s="7"/>
       <c r="W109" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="110" spans="1:23">
@@ -16386,7 +16380,7 @@
         <v>25</v>
       </c>
       <c r="S110" s="9" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="T110" s="9" t="s">
         <v>110</v>
@@ -16398,7 +16392,7 @@
         <v>105</v>
       </c>
       <c r="W110" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -16458,7 +16452,7 @@
       <c r="U111" s="6"/>
       <c r="V111" s="7"/>
       <c r="W111" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="112" spans="1:23">
@@ -16522,7 +16516,7 @@
       <c r="U112" s="6"/>
       <c r="V112" s="7"/>
       <c r="W112" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="113" spans="1:23">
@@ -16590,7 +16584,7 @@
       <c r="U113" s="6"/>
       <c r="V113" s="7"/>
       <c r="W113" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="114" spans="1:23">
@@ -16660,7 +16654,7 @@
       </c>
       <c r="V114" s="7"/>
       <c r="W114" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="115" spans="1:23">
@@ -16732,7 +16726,7 @@
         <v>105</v>
       </c>
       <c r="W115" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="116" spans="1:23">
@@ -16794,7 +16788,7 @@
       <c r="U116" s="6"/>
       <c r="V116" s="7"/>
       <c r="W116" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="117" spans="1:23">
@@ -16858,7 +16852,7 @@
       <c r="U117" s="6"/>
       <c r="V117" s="7"/>
       <c r="W117" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="118" spans="1:23">
@@ -16926,7 +16920,7 @@
       <c r="U118" s="6"/>
       <c r="V118" s="7"/>
       <c r="W118" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="119" spans="1:23">
@@ -16996,7 +16990,7 @@
       </c>
       <c r="V119" s="7"/>
       <c r="W119" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="120" spans="1:23">
@@ -17068,7 +17062,7 @@
         <v>139</v>
       </c>
       <c r="W120" s="134" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="121" spans="1:23">
@@ -17126,7 +17120,7 @@
       <c r="U121" s="6"/>
       <c r="V121" s="7"/>
       <c r="W121" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="122" spans="1:23">
@@ -17188,7 +17182,7 @@
       <c r="U122" s="6"/>
       <c r="V122" s="7"/>
       <c r="W122" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="123" spans="1:23">
@@ -17254,7 +17248,7 @@
       <c r="U123" s="6"/>
       <c r="V123" s="7"/>
       <c r="W123" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="124" spans="1:23">
@@ -17322,7 +17316,7 @@
       <c r="U124" s="6"/>
       <c r="V124" s="7"/>
       <c r="W124" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="125" spans="1:23">
@@ -17394,7 +17388,7 @@
         <v>105</v>
       </c>
       <c r="W125" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="126" spans="1:23">
@@ -17454,7 +17448,7 @@
       <c r="U126" s="6"/>
       <c r="V126" s="7"/>
       <c r="W126" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="127" spans="1:23">
@@ -17516,7 +17510,7 @@
       <c r="U127" s="6"/>
       <c r="V127" s="7"/>
       <c r="W127" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -17576,7 +17570,7 @@
         <v>98</v>
       </c>
       <c r="S128" s="6" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="T128" s="6" t="s">
         <v>50</v>
@@ -17584,7 +17578,7 @@
       <c r="U128" s="6"/>
       <c r="V128" s="7"/>
       <c r="W128" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="129" spans="1:23">
@@ -17654,7 +17648,7 @@
       </c>
       <c r="V129" s="7"/>
       <c r="W129" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="130" spans="1:23">
@@ -17726,7 +17720,7 @@
         <v>70</v>
       </c>
       <c r="W130" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="131" spans="1:23">
@@ -17788,7 +17782,7 @@
       <c r="U131" s="6"/>
       <c r="V131" s="7"/>
       <c r="W131" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="132" spans="1:23">
@@ -17854,7 +17848,7 @@
       <c r="U132" s="6"/>
       <c r="V132" s="7"/>
       <c r="W132" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="133" spans="1:23">
@@ -17922,7 +17916,7 @@
       <c r="U133" s="6"/>
       <c r="V133" s="7"/>
       <c r="W133" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="134" spans="1:23">
@@ -17992,7 +17986,7 @@
       </c>
       <c r="V134" s="7"/>
       <c r="W134" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="135" spans="1:23">
@@ -18064,7 +18058,7 @@
         <v>105</v>
       </c>
       <c r="W135" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="136" spans="1:23">
@@ -19717,7 +19711,7 @@
         <v>108</v>
       </c>
       <c r="P160" s="9" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="Q160" s="9" t="s">
         <v>485</v>
@@ -21071,7 +21065,7 @@
         <v>431</v>
       </c>
       <c r="P180" s="9" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="Q180" s="9" t="s">
         <v>390</v>
@@ -21150,7 +21144,7 @@
       <c r="U181" s="6"/>
       <c r="V181" s="7"/>
       <c r="W181" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="182" spans="1:23">
@@ -21210,7 +21204,7 @@
       <c r="U182" s="6"/>
       <c r="V182" s="7"/>
       <c r="W182" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="183" spans="1:23">
@@ -21278,7 +21272,7 @@
       <c r="U183" s="6"/>
       <c r="V183" s="7"/>
       <c r="W183" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="184" spans="1:23">
@@ -21348,7 +21342,7 @@
       </c>
       <c r="V184" s="10"/>
       <c r="W184" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="185" spans="1:23">
@@ -21412,7 +21406,7 @@
       <c r="U185" s="9"/>
       <c r="V185" s="10"/>
       <c r="W185" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="186" spans="1:23">
@@ -21470,7 +21464,7 @@
       <c r="U186" s="6"/>
       <c r="V186" s="7"/>
       <c r="W186" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="187" spans="1:23">
@@ -21532,7 +21526,7 @@
       <c r="U187" s="6"/>
       <c r="V187" s="7"/>
       <c r="W187" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="188" spans="1:23">
@@ -21600,7 +21594,7 @@
       <c r="U188" s="6"/>
       <c r="V188" s="7"/>
       <c r="W188" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="189" spans="1:23">
@@ -21657,7 +21651,7 @@
         <v>558</v>
       </c>
       <c r="R189" s="9" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="S189" s="9" t="s">
         <v>567</v>
@@ -21670,7 +21664,7 @@
       </c>
       <c r="V189" s="10"/>
       <c r="W189" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="190" spans="1:23">
@@ -21724,7 +21718,7 @@
         <v>37</v>
       </c>
       <c r="Q190" s="9" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="R190" s="9" t="s">
         <v>101</v>
@@ -21736,7 +21730,7 @@
       <c r="U190" s="9"/>
       <c r="V190" s="10"/>
       <c r="W190" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="191" spans="1:23">
@@ -21796,7 +21790,7 @@
       <c r="U191" s="6"/>
       <c r="V191" s="7"/>
       <c r="W191" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="192" spans="1:23">
@@ -21858,7 +21852,7 @@
       <c r="U192" s="6"/>
       <c r="V192" s="7"/>
       <c r="W192" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="193" spans="1:23">
@@ -21926,7 +21920,7 @@
       <c r="U193" s="6"/>
       <c r="V193" s="7"/>
       <c r="W193" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="194" spans="1:23">
@@ -21996,7 +21990,7 @@
       </c>
       <c r="V194" s="10"/>
       <c r="W194" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="195" spans="1:23">
@@ -22062,7 +22056,7 @@
       <c r="U195" s="9"/>
       <c r="V195" s="10"/>
       <c r="W195" s="134" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="196" spans="1:23">
@@ -22122,7 +22116,7 @@
       <c r="U196" s="6"/>
       <c r="V196" s="7"/>
       <c r="W196" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="197" spans="1:23">
@@ -22186,7 +22180,7 @@
       <c r="U197" s="6"/>
       <c r="V197" s="7"/>
       <c r="W197" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="198" spans="1:23">
@@ -22234,7 +22228,7 @@
         <v>612</v>
       </c>
       <c r="O198" s="6" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="P198" s="6" t="s">
         <v>613</v>
@@ -22254,7 +22248,7 @@
       <c r="U198" s="6"/>
       <c r="V198" s="7"/>
       <c r="W198" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="199" spans="1:23">
@@ -22324,7 +22318,7 @@
       </c>
       <c r="V199" s="10"/>
       <c r="W199" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="200" spans="1:23">
@@ -22386,7 +22380,7 @@
       <c r="U200" s="9"/>
       <c r="V200" s="10"/>
       <c r="W200" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="201" spans="1:23">
@@ -22446,7 +22440,7 @@
       <c r="U201" s="6"/>
       <c r="V201" s="7"/>
       <c r="W201" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="202" spans="1:23">
@@ -22510,7 +22504,7 @@
       <c r="U202" s="6"/>
       <c r="V202" s="7"/>
       <c r="W202" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="203" spans="1:23">
@@ -22578,7 +22572,7 @@
       <c r="U203" s="6"/>
       <c r="V203" s="7"/>
       <c r="W203" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="204" spans="1:23">
@@ -22648,7 +22642,7 @@
       </c>
       <c r="V204" s="10"/>
       <c r="W204" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="205" spans="1:23">
@@ -23298,7 +23292,7 @@
       <c r="U214" s="12"/>
       <c r="V214" s="16"/>
       <c r="W214" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="215" spans="1:23">
@@ -23360,7 +23354,7 @@
       <c r="U215" s="6"/>
       <c r="V215" s="7"/>
       <c r="W215" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="216" spans="1:23">
@@ -23428,7 +23422,7 @@
       <c r="U216" s="6"/>
       <c r="V216" s="7"/>
       <c r="W216" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="217" spans="1:23">
@@ -23498,7 +23492,7 @@
       </c>
       <c r="V217" s="10"/>
       <c r="W217" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="218" spans="1:23">
@@ -23558,7 +23552,7 @@
       <c r="U218" s="12"/>
       <c r="V218" s="16"/>
       <c r="W218" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="219" spans="1:23">
@@ -23620,7 +23614,7 @@
       <c r="U219" s="6"/>
       <c r="V219" s="7"/>
       <c r="W219" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="220" spans="1:23">
@@ -23686,7 +23680,7 @@
       <c r="U220" s="6"/>
       <c r="V220" s="7"/>
       <c r="W220" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="221" spans="1:23">
@@ -23756,7 +23750,7 @@
       </c>
       <c r="V221" s="10"/>
       <c r="W221" s="134" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="222" spans="1:23">
@@ -23818,7 +23812,7 @@
       <c r="U222" s="6"/>
       <c r="V222" s="7"/>
       <c r="W222" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="223" spans="1:23">
@@ -23888,7 +23882,7 @@
       </c>
       <c r="V223" s="7"/>
       <c r="W223" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="224" spans="1:23">
@@ -23954,7 +23948,7 @@
       <c r="U224" s="6"/>
       <c r="V224" s="7"/>
       <c r="W224" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="225" spans="1:23">
@@ -24014,7 +24008,7 @@
       <c r="U225" s="6"/>
       <c r="V225" s="7"/>
       <c r="W225" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="226" spans="1:23">
@@ -24080,7 +24074,7 @@
       <c r="U226" s="6"/>
       <c r="V226" s="7"/>
       <c r="W226" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="227" spans="1:23">
@@ -24131,7 +24125,7 @@
         <v>558</v>
       </c>
       <c r="P227" s="6" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="Q227" s="6"/>
       <c r="R227" s="6"/>
@@ -24140,7 +24134,7 @@
       <c r="U227" s="6"/>
       <c r="V227" s="7"/>
       <c r="W227" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="228" spans="1:23">
@@ -24204,7 +24198,7 @@
       <c r="U228" s="6"/>
       <c r="V228" s="7"/>
       <c r="W228" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="229" spans="1:23">
@@ -24272,7 +24266,7 @@
       <c r="U229" s="6"/>
       <c r="V229" s="7"/>
       <c r="W229" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="230" spans="1:23">
@@ -24340,7 +24334,7 @@
       <c r="U230" s="6"/>
       <c r="V230" s="7"/>
       <c r="W230" s="134" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="231" spans="1:23">
@@ -24412,7 +24406,7 @@
         <v>33</v>
       </c>
       <c r="W231" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="232" spans="1:23">
@@ -24552,7 +24546,7 @@
         <v>50</v>
       </c>
       <c r="W233" s="126" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="234" spans="1:23">
@@ -24622,7 +24616,7 @@
       </c>
       <c r="V234" s="7"/>
       <c r="W234" s="126" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="235" spans="1:23">
@@ -24697,7 +24691,7 @@
         <v>Human M</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="C236" s="5" t="s">
         <v>9</v>
@@ -24748,7 +24742,7 @@
       <c r="U236" s="6"/>
       <c r="V236" s="7"/>
       <c r="W236" s="126" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="237" spans="1:23">
@@ -24757,7 +24751,7 @@
         <v>Human F</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="C237" s="5" t="s">
         <v>9</v>
@@ -24808,7 +24802,7 @@
       <c r="U237" s="6"/>
       <c r="V237" s="7"/>
       <c r="W237" s="126" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="238" spans="1:23">
@@ -24870,7 +24864,7 @@
       <c r="U238" s="6"/>
       <c r="V238" s="7"/>
       <c r="W238" s="126" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="239" spans="1:23">
@@ -24932,7 +24926,7 @@
       <c r="U239" s="6"/>
       <c r="V239" s="7"/>
       <c r="W239" s="126" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="240" spans="1:23">
@@ -25052,7 +25046,7 @@
       <c r="U241" s="6"/>
       <c r="V241" s="7"/>
       <c r="W241" s="126" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="242" spans="1:23">
@@ -25061,7 +25055,7 @@
         <v>Hatchling</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>9</v>
@@ -25114,7 +25108,7 @@
       <c r="U242" s="6"/>
       <c r="V242" s="7"/>
       <c r="W242" s="134" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="243" spans="1:23">
@@ -25240,7 +25234,7 @@
       <c r="U244" s="6"/>
       <c r="V244" s="7"/>
       <c r="W244" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="245" spans="1:23">
@@ -25306,7 +25300,7 @@
       <c r="U245" s="6"/>
       <c r="V245" s="7"/>
       <c r="W245" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="246" spans="1:23">
@@ -25372,7 +25366,7 @@
       <c r="U246" s="6"/>
       <c r="V246" s="7"/>
       <c r="W246" s="126" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="247" spans="1:23">
@@ -25440,7 +25434,7 @@
       <c r="U247" s="6"/>
       <c r="V247" s="7"/>
       <c r="W247" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="248" spans="1:23">
@@ -25491,7 +25485,7 @@
         <v>770</v>
       </c>
       <c r="P248" s="6" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="Q248" s="6" t="s">
         <v>441</v>
@@ -25506,7 +25500,7 @@
       <c r="U248" s="6"/>
       <c r="V248" s="7"/>
       <c r="W248" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="249" spans="1:23">
@@ -25566,13 +25560,13 @@
         <v>268</v>
       </c>
       <c r="S249" s="6" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="T249" s="6"/>
       <c r="U249" s="6"/>
       <c r="V249" s="7"/>
       <c r="W249" s="126" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="250" spans="1:23">
@@ -25628,7 +25622,7 @@
       <c r="U250" s="6"/>
       <c r="V250" s="7"/>
       <c r="W250" s="126" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="251" spans="1:23">
@@ -25724,7 +25718,7 @@
       </c>
       <c r="P252" s="126"/>
       <c r="W252" s="126" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="253" spans="1:23">
@@ -25733,7 +25727,7 @@
         <v>SuperJerk</v>
       </c>
       <c r="B253" s="124" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="C253">
         <v>3</v>
@@ -25775,7 +25769,7 @@
         <v>135</v>
       </c>
       <c r="W253" s="126" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
   </sheetData>
@@ -35979,7 +35973,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R154" sqref="R154"/>
+      <selection pane="bottomLeft" activeCell="Y122" sqref="Y122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36011,7 +36005,7 @@
         <v>1642</v>
       </c>
       <c r="E1" s="135" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="F1" s="88" t="s">
         <v>1643</v>
@@ -36059,7 +36053,7 @@
         <v>2369</v>
       </c>
       <c r="W1" s="121" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="X1" s="121" t="s">
         <v>2362</v>
@@ -36651,7 +36645,7 @@
         <v>2305</v>
       </c>
       <c r="U11" t="s">
-        <v>2371</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="12" spans="1:27" hidden="1">
@@ -37025,7 +37019,7 @@
         <v>2305</v>
       </c>
       <c r="AA17" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1">
@@ -37422,7 +37416,7 @@
         <v>2306</v>
       </c>
       <c r="Y24" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="Z24">
         <v>90</v>
@@ -37592,7 +37586,7 @@
       <c r="T27" t="s">
         <v>2308</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="X27" t="s">
         <v>1766</v>
       </c>
     </row>
@@ -37646,7 +37640,7 @@
       <c r="T28" t="s">
         <v>2308</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="X28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -37951,7 +37945,7 @@
         <v>2309</v>
       </c>
       <c r="U33" t="s">
-        <v>2371</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="34" spans="1:25" hidden="1">
@@ -38463,7 +38457,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="43" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
@@ -38957,7 +38951,7 @@
         <v>1816</v>
       </c>
       <c r="U52" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="53" spans="1:25" hidden="1">
@@ -39366,8 +39360,11 @@
       <c r="T61" t="s">
         <v>2308</v>
       </c>
+      <c r="X61" t="s">
+        <v>2573</v>
+      </c>
       <c r="Y61" t="s">
-        <v>2574</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:25" hidden="1">
@@ -39420,7 +39417,7 @@
       <c r="T62" t="s">
         <v>2308</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="X62" t="s">
         <v>482</v>
       </c>
     </row>
@@ -39642,7 +39639,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="68" spans="1:27" hidden="1">
+    <row r="68" spans="1:27">
       <c r="A68" t="str">
         <f t="shared" si="6"/>
         <v>Whip</v>
@@ -39698,13 +39695,13 @@
         <v>2305</v>
       </c>
       <c r="Y68" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="Z68">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:27" hidden="1">
+    <row r="69" spans="1:27">
       <c r="A69" t="str">
         <f t="shared" si="6"/>
         <v>Blitz Whip</v>
@@ -39761,13 +39758,13 @@
         <v>2305</v>
       </c>
       <c r="Y69" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="Z69">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:27" hidden="1">
+    <row r="70" spans="1:27">
       <c r="A70" t="str">
         <f t="shared" si="6"/>
         <v>ChainSaw</v>
@@ -39819,10 +39816,10 @@
         <v>2305</v>
       </c>
       <c r="Y70" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" hidden="1">
       <c r="A71" t="str">
         <f t="shared" si="6"/>
         <v>Counter</v>
@@ -40269,7 +40266,7 @@
         <v>Roundhouse Art</v>
       </c>
       <c r="C78" s="94" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="D78" s="96" t="s">
         <v>2317</v>
@@ -40315,7 +40312,7 @@
         <v>2305</v>
       </c>
       <c r="AA78" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="79" spans="1:27" hidden="1">
@@ -40681,7 +40678,7 @@
         <v>0</v>
       </c>
       <c r="K85" s="43" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="L85" s="19"/>
       <c r="M85" s="19"/>
@@ -41665,7 +41662,7 @@
         <v>2305</v>
       </c>
       <c r="U102" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="103" spans="1:27" hidden="1">
@@ -41788,7 +41785,7 @@
         <v>2305</v>
       </c>
       <c r="AA104" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="105" spans="1:27" hidden="1">
@@ -42008,7 +42005,7 @@
         <v>5</v>
       </c>
       <c r="S108" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="T108" t="s">
         <v>2307</v>
@@ -42186,7 +42183,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="112" spans="1:27" hidden="1">
+    <row r="112" spans="1:27">
       <c r="A112" t="str">
         <f t="shared" si="6"/>
         <v>Hyper Cannon</v>
@@ -42328,7 +42325,7 @@
         <v>1816</v>
       </c>
       <c r="U114" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="115" spans="1:26" hidden="1">
@@ -42570,7 +42567,7 @@
         <v>2306</v>
       </c>
       <c r="U119" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="Y119" t="s">
         <v>572</v>
@@ -42629,8 +42626,8 @@
       <c r="T120" t="s">
         <v>2311</v>
       </c>
-      <c r="Y120" t="s">
-        <v>2573</v>
+      <c r="X120" t="s">
+        <v>2572</v>
       </c>
     </row>
     <row r="121" spans="1:26" hidden="1">
@@ -42678,7 +42675,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="122" spans="1:26" hidden="1">
+    <row r="122" spans="1:26">
       <c r="A122" t="str">
         <f t="shared" si="6"/>
         <v>Selfix</v>
@@ -42711,7 +42708,7 @@
         <v>0</v>
       </c>
       <c r="K122" s="43" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="P122" s="5">
         <v>1</v>
@@ -42720,13 +42717,13 @@
         <v>1816</v>
       </c>
       <c r="Y122" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="Z122">
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:26" hidden="1">
+    <row r="123" spans="1:26">
       <c r="A123" t="str">
         <f t="shared" si="6"/>
         <v>Seven Sword</v>
@@ -42761,7 +42758,7 @@
         <v>0</v>
       </c>
       <c r="K123" s="43" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="L123" s="19"/>
       <c r="M123" s="19"/>
@@ -43556,7 +43553,7 @@
         <v>2305</v>
       </c>
       <c r="AA137" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="138" spans="1:27" hidden="1">
@@ -43724,7 +43721,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="141" spans="1:27" hidden="1">
+    <row r="141" spans="1:27">
       <c r="A141" t="str">
         <f t="shared" si="11"/>
         <v>W-Pincer</v>
@@ -43780,7 +43777,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="142" spans="1:27" hidden="1">
+    <row r="142" spans="1:27">
       <c r="A142" t="str">
         <f t="shared" si="11"/>
         <v>W-Attack</v>
@@ -43838,7 +43835,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="143" spans="1:27" hidden="1">
+    <row r="143" spans="1:27">
       <c r="A143" t="str">
         <f t="shared" si="11"/>
         <v>4-Heads</v>
@@ -43896,7 +43893,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="144" spans="1:27" hidden="1">
+    <row r="144" spans="1:27">
       <c r="A144" t="str">
         <f t="shared" si="11"/>
         <v>8-Legs</v>
@@ -43954,7 +43951,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="145" spans="1:27" hidden="1">
+    <row r="145" spans="1:27">
       <c r="A145" t="str">
         <f t="shared" si="11"/>
         <v>Touch</v>
@@ -44013,7 +44010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="1:27" hidden="1">
+    <row r="146" spans="1:27">
       <c r="A146" t="str">
         <f t="shared" si="11"/>
         <v>Saw</v>
@@ -44063,10 +44060,10 @@
         <v>2305</v>
       </c>
       <c r="Y146" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="147" spans="1:27" hidden="1">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27">
       <c r="A147" t="str">
         <f t="shared" si="11"/>
         <v>Dissolve</v>
@@ -44125,7 +44122,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="148" spans="1:27" hidden="1">
+    <row r="148" spans="1:27">
       <c r="A148" t="str">
         <f t="shared" si="11"/>
         <v>Absorb</v>
@@ -44387,7 +44384,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="153" spans="1:27">
+    <row r="153" spans="1:27" hidden="1">
       <c r="A153" t="str">
         <f t="shared" si="11"/>
         <v>Backlash</v>
@@ -44397,7 +44394,7 @@
         <v>Backlash</v>
       </c>
       <c r="C153" s="94" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="D153" s="96"/>
       <c r="E153" s="136">
@@ -44440,10 +44437,10 @@
         <v>121</v>
       </c>
       <c r="AA153" t="s">
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="154" spans="1:27">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="154" spans="1:27" hidden="1">
       <c r="A154" t="str">
         <f t="shared" si="11"/>
         <v>Burning</v>
@@ -44499,7 +44496,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="155" spans="1:27" hidden="1">
+    <row r="155" spans="1:27">
       <c r="A155" t="str">
         <f t="shared" si="11"/>
         <v>2-Swords</v>
@@ -44555,7 +44552,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="156" spans="1:27" hidden="1">
+    <row r="156" spans="1:27">
       <c r="A156" t="str">
         <f t="shared" si="11"/>
         <v>2-Tusks</v>
@@ -44611,7 +44608,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="157" spans="1:27" hidden="1">
+    <row r="157" spans="1:27">
       <c r="A157" t="str">
         <f t="shared" si="11"/>
         <v>3-Heads</v>
@@ -44669,7 +44666,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="158" spans="1:27" hidden="1">
+    <row r="158" spans="1:27">
       <c r="A158" t="str">
         <f t="shared" si="11"/>
         <v>3-Horns</v>
@@ -44727,7 +44724,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="159" spans="1:27" hidden="1">
+    <row r="159" spans="1:27">
       <c r="A159" t="str">
         <f t="shared" si="11"/>
         <v>6-Arms</v>
@@ -44783,7 +44780,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="160" spans="1:27" hidden="1">
+    <row r="160" spans="1:27">
       <c r="A160" t="str">
         <f t="shared" si="11"/>
         <v>Critical</v>
@@ -45012,7 +45009,7 @@
         <v>MegaCure</v>
       </c>
       <c r="B164" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="C164" s="94" t="s">
         <v>75</v>
@@ -45063,10 +45060,10 @@
         <v>74</v>
       </c>
       <c r="AA164" t="s">
-        <v>2375</v>
-      </c>
-    </row>
-    <row r="165" spans="1:27" hidden="1">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="165" spans="1:27">
       <c r="A165" t="str">
         <f t="shared" si="11"/>
         <v>W-Kick</v>
@@ -45387,7 +45384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:27">
+    <row r="171" spans="1:27" hidden="1">
       <c r="A171" t="str">
         <f t="shared" si="11"/>
         <v>P-Skin</v>
@@ -45440,7 +45437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:27">
+    <row r="172" spans="1:27" hidden="1">
       <c r="A172" t="str">
         <f t="shared" si="11"/>
         <v>ParaSkin</v>
@@ -45546,7 +45543,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="174" spans="1:27">
+    <row r="174" spans="1:27" hidden="1">
       <c r="A174" t="str">
         <f t="shared" si="11"/>
         <v>StonSkin</v>
@@ -45945,7 +45942,7 @@
         <v>Lightning</v>
       </c>
       <c r="C181" s="94" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="D181" s="96"/>
       <c r="E181" s="136">
@@ -46150,7 +46147,7 @@
         <v>2309</v>
       </c>
       <c r="U184" t="s">
-        <v>2371</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="185" spans="1:24" hidden="1">
@@ -46206,7 +46203,7 @@
         <v>2309</v>
       </c>
       <c r="U185" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="186" spans="1:24" hidden="1">
@@ -46318,7 +46315,7 @@
         <v>2309</v>
       </c>
       <c r="U187" t="s">
-        <v>2371</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="188" spans="1:24" hidden="1">
@@ -46649,7 +46646,7 @@
         <v>DeathGaze</v>
       </c>
       <c r="C194" s="94" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="D194" s="96"/>
       <c r="E194" s="136">
@@ -46692,7 +46689,7 @@
         <v>2370</v>
       </c>
       <c r="AA194" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="195" spans="1:27" hidden="1">
@@ -46970,7 +46967,7 @@
         <v>EvilEye</v>
       </c>
       <c r="C200" s="94" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="D200" s="96"/>
       <c r="E200" s="136">
@@ -47013,7 +47010,7 @@
         <v>1766</v>
       </c>
       <c r="AA200" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="201" spans="1:27" hidden="1">
@@ -47269,7 +47266,7 @@
         <v>1</v>
       </c>
       <c r="S205" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="T205" t="s">
         <v>2309</v>
@@ -47322,7 +47319,7 @@
         <v>1</v>
       </c>
       <c r="S206" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="T206" t="s">
         <v>2309</v>
@@ -47375,7 +47372,7 @@
         <v>2012</v>
       </c>
       <c r="S207" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="T207" t="s">
         <v>2309</v>
@@ -47428,7 +47425,7 @@
         <v>1</v>
       </c>
       <c r="S208" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="T208" t="s">
         <v>2305</v>
@@ -47481,7 +47478,7 @@
         <v>1</v>
       </c>
       <c r="S209" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="T209" t="s">
         <v>2305</v>
@@ -47534,7 +47531,7 @@
         <v>2012</v>
       </c>
       <c r="S210" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="T210" t="s">
         <v>2307</v>
@@ -47761,7 +47758,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="215" spans="1:25" hidden="1">
+    <row r="215" spans="1:25">
       <c r="A215" t="str">
         <f t="shared" si="14"/>
         <v>Steal</v>
@@ -47814,7 +47811,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="216" spans="1:25" hidden="1">
+    <row r="216" spans="1:25">
       <c r="A216" t="str">
         <f t="shared" si="14"/>
         <v>Explode</v>
@@ -47867,7 +47864,7 @@
         <v>0</v>
       </c>
       <c r="Y216" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="217" spans="1:25" hidden="1">
@@ -48214,7 +48211,7 @@
         <v>1</v>
       </c>
       <c r="S223" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="T223" t="s">
         <v>2307</v>
@@ -48462,7 +48459,7 @@
         <v>2352</v>
       </c>
       <c r="U228" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="229" spans="1:27" hidden="1">
@@ -48609,7 +48606,7 @@
         <v>2352</v>
       </c>
       <c r="U231" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="232" spans="1:27" hidden="1">
@@ -48759,7 +48756,7 @@
         <v>159</v>
       </c>
       <c r="Y234" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="235" spans="1:27" hidden="1">
@@ -48811,7 +48808,7 @@
         <v>441</v>
       </c>
       <c r="Y235" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="236" spans="1:27" hidden="1">
@@ -48863,7 +48860,7 @@
         <v>242</v>
       </c>
       <c r="Y236" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="237" spans="1:27" hidden="1">
@@ -48999,7 +48996,7 @@
         <v>2352</v>
       </c>
       <c r="U239" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="240" spans="1:27" hidden="1">
@@ -49617,10 +49614,10 @@
         <v>2305</v>
       </c>
       <c r="AA252" t="s">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="253" spans="1:27" hidden="1">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="253" spans="1:27">
       <c r="A253" t="str">
         <f t="shared" si="14"/>
         <v>Vampic Sword</v>
@@ -49747,11 +49744,8 @@
       <c r="W254">
         <v>100</v>
       </c>
-      <c r="Y254" t="s">
-        <v>2584</v>
-      </c>
-    </row>
-    <row r="255" spans="1:27">
+    </row>
+    <row r="255" spans="1:27" hidden="1">
       <c r="A255" t="str">
         <f t="shared" si="14"/>
         <v>Revenge Sword</v>
@@ -49932,7 +49926,7 @@
         <v>2305</v>
       </c>
       <c r="AA257" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="258" spans="1:27" hidden="1">
@@ -49957,17 +49951,25 @@
         <v>2352</v>
       </c>
       <c r="U258" t="s">
+        <v>2574</v>
+      </c>
+      <c r="AA258" t="s">
         <v>2575</v>
-      </c>
-      <c r="AA258" t="s">
-        <v>2576</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AA258" xr:uid="{00000000-0009-0000-0000-000003000000}">
-    <filterColumn colId="19">
+    <filterColumn colId="24">
       <filters>
-        <filter val="Counter"/>
+        <filter val="Absorb"/>
+        <filter val="Critical"/>
+        <filter val="Cut"/>
+        <filter val="Erase"/>
+        <filter val="Multi"/>
+        <filter val="Regen"/>
+        <filter val="Sacrifice"/>
+        <filter val="Steal"/>
+        <filter val="WindUp"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:AA257">
@@ -63053,7 +63055,7 @@
     <row r="110" spans="1:2">
       <c r="A110" s="101"/>
       <c r="B110" s="101" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -63579,7 +63581,7 @@
     <row r="190" spans="1:2">
       <c r="A190" s="101"/>
       <c r="B190" s="101" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -64812,7 +64814,7 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="134" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="C1" s="137" t="s">
         <v>2345</v>
@@ -64872,7 +64874,7 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="134" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="B2" s="117" t="e">
         <f>VLOOKUP(C2,Weapon!B1:Z258,2,FALSE)</f>
@@ -64900,7 +64902,7 @@
         <v>77</v>
       </c>
       <c r="J2" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="K2" s="134" t="s">
         <v>599</v>
@@ -64938,7 +64940,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="134" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="B3" s="117" t="e">
         <f>VLOOKUP(C3,#REF!,2,FALSE)</f>
@@ -64966,7 +64968,7 @@
         <v>77</v>
       </c>
       <c r="J3" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="K3" s="134" t="s">
         <v>599</v>
@@ -65005,7 +65007,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="134" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="B4" s="117" t="e">
         <f>VLOOKUP(C4,#REF!,2,FALSE)</f>
@@ -65071,7 +65073,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="134" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="B5" s="117" t="e">
         <f>VLOOKUP(C5,#REF!,2,FALSE)</f>
@@ -65105,7 +65107,7 @@
         <v>57</v>
       </c>
       <c r="L5" s="117" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="M5" s="139">
         <v>7</v>
@@ -65129,7 +65131,7 @@
         <v>1681</v>
       </c>
       <c r="T5" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="U5" s="134" t="s">
         <v>57</v>
@@ -65137,7 +65139,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="134" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="B6" s="117" t="e">
         <f>VLOOKUP(C6,#REF!,2,FALSE)</f>
@@ -65192,7 +65194,7 @@
         <v>1688</v>
       </c>
       <c r="S6" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="T6" s="134" t="s">
         <v>1689</v>
@@ -65203,7 +65205,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="134" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="B7" s="117" t="e">
         <f>VLOOKUP(C7,#REF!,2,FALSE)</f>
@@ -65269,7 +65271,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="134" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="B8" s="117" t="e">
         <f>VLOOKUP(C8,#REF!,2,FALSE)</f>
@@ -65335,7 +65337,7 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="134" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="B9" s="117" t="e">
         <f>VLOOKUP(C9,#REF!,2,FALSE)</f>
@@ -65363,7 +65365,7 @@
         <v>77</v>
       </c>
       <c r="J9" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="K9" s="134" t="s">
         <v>599</v>
@@ -65401,7 +65403,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="134" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="B10" s="117" t="e">
         <f>VLOOKUP(C10,#REF!,2,FALSE)</f>
@@ -65467,7 +65469,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="134" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="B11" s="117" t="e">
         <f>VLOOKUP(C11,#REF!,2,FALSE)</f>
@@ -65492,7 +65494,7 @@
         <v>545</v>
       </c>
       <c r="I11" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="J11" s="134" t="s">
         <v>1725</v>
@@ -65501,7 +65503,7 @@
         <v>57</v>
       </c>
       <c r="L11" s="117" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="M11" s="139">
         <v>19</v>
@@ -65533,7 +65535,7 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="134" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="B12" s="117" t="e">
         <f>VLOOKUP(C12,#REF!,2,FALSE)</f>
@@ -65599,7 +65601,7 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="134" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="B13" s="117" t="e">
         <f>VLOOKUP(C13,#REF!,2,FALSE)</f>
@@ -65624,7 +65626,7 @@
         <v>714</v>
       </c>
       <c r="I13" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="J13" s="134" t="s">
         <v>1733</v>
@@ -65665,7 +65667,7 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="134" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="B14" s="117" t="e">
         <f>VLOOKUP(C14,#REF!,2,FALSE)</f>
@@ -65731,7 +65733,7 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="134" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="B15" s="117" t="e">
         <f>VLOOKUP(C15,#REF!,2,FALSE)</f>
@@ -65797,7 +65799,7 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="134" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="B16" s="117" t="e">
         <f>VLOOKUP(C16,#REF!,2,FALSE)</f>
@@ -65863,7 +65865,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="134" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="B17" s="117" t="e">
         <f>VLOOKUP(C17,#REF!,2,FALSE)</f>
@@ -65885,7 +65887,7 @@
         <v>128</v>
       </c>
       <c r="H17" s="134" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="I17" s="134" t="s">
         <v>776</v>
@@ -65897,7 +65899,7 @@
         <v>1500</v>
       </c>
       <c r="L17" s="117" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="M17" s="139">
         <v>31</v>
@@ -65929,7 +65931,7 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="134" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="B18" s="117" t="e">
         <f>VLOOKUP(C18,#REF!,2,FALSE)</f>
@@ -65995,7 +65997,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="134" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="B19" s="117" t="e">
         <f>VLOOKUP(C19,#REF!,2,FALSE)</f>
@@ -66050,7 +66052,7 @@
         <v>1778</v>
       </c>
       <c r="S19" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T19" s="134" t="s">
         <v>1733</v>
@@ -66061,7 +66063,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="134" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="B20" s="117" t="e">
         <f>VLOOKUP(C20,#REF!,2,FALSE)</f>
@@ -66116,7 +66118,7 @@
         <v>1678</v>
       </c>
       <c r="S20" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="T20" s="134" t="s">
         <v>1784</v>
@@ -66127,7 +66129,7 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="134" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="B21" s="117" t="e">
         <f>VLOOKUP(C21,#REF!,2,FALSE)</f>
@@ -66188,12 +66190,12 @@
         <v>487</v>
       </c>
       <c r="U21" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="134" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B22" s="117" t="e">
         <f>VLOOKUP(C22,#REF!,2,FALSE)</f>
@@ -66259,7 +66261,7 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="134" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="B23" s="117" t="e">
         <f>VLOOKUP(C23,#REF!,2,FALSE)</f>
@@ -66325,7 +66327,7 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="134" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="B24" s="117" t="e">
         <f>VLOOKUP(C24,#REF!,2,FALSE)</f>
@@ -66391,7 +66393,7 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="134" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="B25" s="117" t="e">
         <f>VLOOKUP(C25,#REF!,2,FALSE)</f>
@@ -66457,7 +66459,7 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="134" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="B26" s="117" t="e">
         <f>VLOOKUP(C26,#REF!,2,FALSE)</f>
@@ -66488,7 +66490,7 @@
         <v>1684</v>
       </c>
       <c r="K26" s="134" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="L26" s="117" t="s">
         <v>699</v>
@@ -66523,7 +66525,7 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="134" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="B27" s="117" t="e">
         <f>VLOOKUP(C27,#REF!,2,FALSE)</f>
@@ -66589,7 +66591,7 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="134" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="B28" s="117" t="e">
         <f>VLOOKUP(C28,#REF!,2,FALSE)</f>
@@ -66605,7 +66607,7 @@
         <v>77</v>
       </c>
       <c r="F28" s="134" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="G28" s="134" t="s">
         <v>77</v>
@@ -66655,7 +66657,7 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="134" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="B29" s="117" t="e">
         <f>VLOOKUP(C29,#REF!,2,FALSE)</f>
@@ -66721,7 +66723,7 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="134" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="B30" s="117" t="e">
         <f>VLOOKUP(C30,#REF!,2,FALSE)</f>
@@ -66737,7 +66739,7 @@
         <v>77</v>
       </c>
       <c r="F30" s="134" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="G30" s="134" t="s">
         <v>77</v>
@@ -66755,7 +66757,7 @@
         <v>77</v>
       </c>
       <c r="L30" s="117" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="M30" s="139">
         <v>57</v>
@@ -66767,7 +66769,7 @@
         <v>77</v>
       </c>
       <c r="P30" s="134" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="Q30" s="134" t="s">
         <v>77</v>
@@ -66787,7 +66789,7 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="134" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="B31" s="117" t="e">
         <f>VLOOKUP(C31,#REF!,2,FALSE)</f>
@@ -66853,7 +66855,7 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="134" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="B32" s="117" t="e">
         <f>VLOOKUP(C32,#REF!,2,FALSE)</f>
@@ -66919,7 +66921,7 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="134" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="B33" s="117" t="e">
         <f>VLOOKUP(C33,#REF!,2,FALSE)</f>
@@ -66935,7 +66937,7 @@
         <v>77</v>
       </c>
       <c r="F33" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="G33" s="134" t="s">
         <v>77</v>
@@ -66953,7 +66955,7 @@
         <v>77</v>
       </c>
       <c r="L33" s="117" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="M33" s="139">
         <v>63</v>
@@ -66985,7 +66987,7 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="134" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="B34" s="117" t="e">
         <f>VLOOKUP(C34,#REF!,2,FALSE)</f>
@@ -67051,7 +67053,7 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="134" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="B35" s="117" t="e">
         <f>VLOOKUP(C35,#REF!,2,FALSE)</f>
@@ -67085,7 +67087,7 @@
         <v>1500</v>
       </c>
       <c r="L35" s="117" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="M35" s="139">
         <v>67</v>
@@ -67117,7 +67119,7 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="134" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="B36" s="117" t="e">
         <f>VLOOKUP(C36,#REF!,2,FALSE)</f>
@@ -67151,7 +67153,7 @@
         <v>1500</v>
       </c>
       <c r="L36" s="117" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="M36" s="139">
         <v>69</v>
@@ -67183,7 +67185,7 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="134" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="B37" s="117" t="e">
         <f>VLOOKUP(C37,#REF!,2,FALSE)</f>
@@ -67217,7 +67219,7 @@
         <v>1500</v>
       </c>
       <c r="L37" s="117" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="M37" s="139">
         <v>71</v>
@@ -67249,7 +67251,7 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="134" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="B38" s="117" t="e">
         <f>VLOOKUP(C38,#REF!,2,FALSE)</f>
@@ -67277,7 +67279,7 @@
         <v>776</v>
       </c>
       <c r="J38" s="134" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="K38" s="134" t="s">
         <v>182</v>
@@ -67315,7 +67317,7 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="134" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B39" s="117" t="e">
         <f>VLOOKUP(C39,#REF!,2,FALSE)</f>
@@ -67343,7 +67345,7 @@
         <v>1667</v>
       </c>
       <c r="J39" s="134" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="K39" s="134" t="s">
         <v>523</v>
@@ -67373,7 +67375,7 @@
         <v>77</v>
       </c>
       <c r="T39" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="U39" s="134" t="s">
         <v>334</v>
@@ -67381,7 +67383,7 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="134" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="B40" s="117" t="e">
         <f>VLOOKUP(C40,#REF!,2,FALSE)</f>
@@ -67409,7 +67411,7 @@
         <v>1801</v>
       </c>
       <c r="J40" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="K40" s="134" t="s">
         <v>545</v>
@@ -67436,10 +67438,10 @@
         <v>465</v>
       </c>
       <c r="S40" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T40" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="U40" s="134" t="s">
         <v>545</v>
@@ -67447,7 +67449,7 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="134" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="B41" s="117" t="e">
         <f>VLOOKUP(C41,#REF!,2,FALSE)</f>
@@ -67472,16 +67474,16 @@
         <v>27</v>
       </c>
       <c r="I41" s="134" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="J41" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="K41" s="134" t="s">
         <v>545</v>
       </c>
       <c r="L41" s="117" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="M41" s="139">
         <v>79</v>
@@ -67505,7 +67507,7 @@
         <v>27</v>
       </c>
       <c r="T41" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="U41" s="134" t="s">
         <v>334</v>
@@ -67513,7 +67515,7 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="134" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="B42" s="117" t="e">
         <f>VLOOKUP(C42,#REF!,2,FALSE)</f>
@@ -67547,7 +67549,7 @@
         <v>334</v>
       </c>
       <c r="L42" s="117" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="M42" s="139">
         <v>81</v>
@@ -67579,7 +67581,7 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="134" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="B43" s="117" t="e">
         <f>VLOOKUP(C43,#REF!,2,FALSE)</f>
@@ -67613,7 +67615,7 @@
         <v>334</v>
       </c>
       <c r="L43" s="117" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="M43" s="139">
         <v>83</v>
@@ -67634,7 +67636,7 @@
         <v>1007</v>
       </c>
       <c r="S43" s="134" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="T43" s="134" t="s">
         <v>1879</v>
@@ -67645,7 +67647,7 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="134" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="B44" s="117" t="e">
         <f>VLOOKUP(C44,#REF!,2,FALSE)</f>
@@ -67711,7 +67713,7 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="134" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="B45" s="117" t="e">
         <f>VLOOKUP(C45,#REF!,2,FALSE)</f>
@@ -67777,7 +67779,7 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="134" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="B46" s="117" t="e">
         <f>VLOOKUP(C46,#REF!,2,FALSE)</f>
@@ -67843,7 +67845,7 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="134" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="B47" s="117" t="e">
         <f>VLOOKUP(C47,#REF!,2,FALSE)</f>
@@ -67871,7 +67873,7 @@
         <v>77</v>
       </c>
       <c r="J47" s="134" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="K47" s="134" t="s">
         <v>35</v>
@@ -67901,7 +67903,7 @@
         <v>77</v>
       </c>
       <c r="T47" s="134" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="U47" s="134" t="s">
         <v>696</v>
@@ -67909,7 +67911,7 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="134" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="B48" s="117" t="e">
         <f>VLOOKUP(C48,#REF!,2,FALSE)</f>
@@ -67931,7 +67933,7 @@
         <v>200</v>
       </c>
       <c r="H48" s="134" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="I48" s="134" t="s">
         <v>77</v>
@@ -67967,7 +67969,7 @@
         <v>77</v>
       </c>
       <c r="T48" s="134" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="U48" s="134" t="s">
         <v>35</v>
@@ -67975,7 +67977,7 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="134" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="B49" s="117" t="e">
         <f>VLOOKUP(C49,#REF!,2,FALSE)</f>
@@ -68041,7 +68043,7 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" s="134" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="B50" s="117" t="e">
         <f>VLOOKUP(C50,#REF!,2,FALSE)</f>
@@ -68063,10 +68065,10 @@
         <v>446</v>
       </c>
       <c r="H50" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="I50" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="J50" s="134" t="s">
         <v>1681</v>
@@ -68096,7 +68098,7 @@
         <v>1778</v>
       </c>
       <c r="S50" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T50" s="134" t="s">
         <v>1912</v>
@@ -68107,7 +68109,7 @@
     </row>
     <row r="51" spans="1:21">
       <c r="A51" s="134" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="B51" s="117" t="e">
         <f>VLOOKUP(C51,#REF!,2,FALSE)</f>
@@ -68173,7 +68175,7 @@
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="134" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="B52" s="117" t="e">
         <f>VLOOKUP(C52,#REF!,2,FALSE)</f>
@@ -68207,7 +68209,7 @@
         <v>77</v>
       </c>
       <c r="L52" s="117" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="M52" s="139">
         <v>101</v>
@@ -68239,7 +68241,7 @@
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="134" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="B53" s="117" t="e">
         <f>VLOOKUP(C53,#REF!,2,FALSE)</f>
@@ -68267,7 +68269,7 @@
         <v>77</v>
       </c>
       <c r="J53" s="134" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="K53" s="134" t="s">
         <v>1714</v>
@@ -68297,7 +68299,7 @@
         <v>465</v>
       </c>
       <c r="T53" s="134" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="U53" s="134" t="s">
         <v>163</v>
@@ -68305,7 +68307,7 @@
     </row>
     <row r="54" spans="1:21">
       <c r="A54" s="134" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="B54" s="117" t="e">
         <f>VLOOKUP(C54,#REF!,2,FALSE)</f>
@@ -68330,7 +68332,7 @@
         <v>523</v>
       </c>
       <c r="I54" s="134" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="J54" s="134" t="s">
         <v>460</v>
@@ -68357,10 +68359,10 @@
         <v>545</v>
       </c>
       <c r="R54" s="134" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="S54" s="134" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="T54" s="134" t="s">
         <v>1891</v>
@@ -68371,7 +68373,7 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" s="134" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="B55" s="117" t="e">
         <f>VLOOKUP(C55,#REF!,2,FALSE)</f>
@@ -68405,7 +68407,7 @@
         <v>57</v>
       </c>
       <c r="L55" s="117" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="M55" s="139">
         <v>107</v>
@@ -68437,7 +68439,7 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" s="134" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="B56" s="117" t="e">
         <f>VLOOKUP(C56,#REF!,2,FALSE)</f>
@@ -68503,7 +68505,7 @@
     </row>
     <row r="57" spans="1:21">
       <c r="A57" s="134" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="B57" s="117" t="e">
         <f>VLOOKUP(C57,#REF!,2,FALSE)</f>
@@ -68569,7 +68571,7 @@
     </row>
     <row r="58" spans="1:21">
       <c r="A58" s="134" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="B58" s="117" t="e">
         <f>VLOOKUP(C58,#REF!,2,FALSE)</f>
@@ -68627,7 +68629,7 @@
         <v>188</v>
       </c>
       <c r="T58" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="U58" s="134" t="s">
         <v>334</v>
@@ -68635,7 +68637,7 @@
     </row>
     <row r="59" spans="1:21">
       <c r="A59" s="134" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="B59" s="117" t="e">
         <f>VLOOKUP(C59,#REF!,2,FALSE)</f>
@@ -68701,7 +68703,7 @@
     </row>
     <row r="60" spans="1:21">
       <c r="A60" s="134" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="B60" s="117" t="e">
         <f>VLOOKUP(C60,#REF!,2,FALSE)</f>
@@ -68767,7 +68769,7 @@
     </row>
     <row r="61" spans="1:21">
       <c r="A61" s="134" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="B61" s="117" t="e">
         <f>VLOOKUP(C61,#REF!,2,FALSE)</f>
@@ -68801,7 +68803,7 @@
         <v>77</v>
       </c>
       <c r="L61" s="117" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="M61" s="139">
         <v>119</v>
@@ -68833,7 +68835,7 @@
     </row>
     <row r="62" spans="1:21">
       <c r="A62" s="134" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="B62" s="117" t="e">
         <f>VLOOKUP(C62,#REF!,2,FALSE)</f>
@@ -68867,7 +68869,7 @@
         <v>1500</v>
       </c>
       <c r="L62" s="117" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="M62" s="139">
         <v>121</v>
@@ -68899,7 +68901,7 @@
     </row>
     <row r="63" spans="1:21">
       <c r="A63" s="134" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="B63" s="117" t="e">
         <f>VLOOKUP(C63,#REF!,2,FALSE)</f>
@@ -68951,10 +68953,10 @@
         <v>696</v>
       </c>
       <c r="R63" s="134" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="S63" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T63" s="134" t="s">
         <v>460</v>
@@ -68965,7 +68967,7 @@
     </row>
     <row r="64" spans="1:21">
       <c r="A64" s="134" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="B64" s="117" t="e">
         <f>VLOOKUP(C64,#REF!,2,FALSE)</f>
@@ -69031,7 +69033,7 @@
     </row>
     <row r="65" spans="1:21">
       <c r="A65" s="134" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="B65" s="117" t="e">
         <f>VLOOKUP(C65,#REF!,2,FALSE)</f>
@@ -69097,7 +69099,7 @@
     </row>
     <row r="66" spans="1:21">
       <c r="A66" s="134" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="B66" s="117" t="e">
         <f>VLOOKUP(C66,#REF!,2,FALSE)</f>
@@ -69125,7 +69127,7 @@
         <v>77</v>
       </c>
       <c r="J66" s="134" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="K66" s="134" t="s">
         <v>334</v>
@@ -69163,7 +69165,7 @@
     </row>
     <row r="67" spans="1:21">
       <c r="A67" s="134" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="B67" s="117" t="e">
         <f>VLOOKUP(C67,#REF!,2,FALSE)</f>
@@ -69229,7 +69231,7 @@
     </row>
     <row r="68" spans="1:21">
       <c r="A68" s="134" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="B68" s="117" t="e">
         <f>VLOOKUP(C68,#REF!,2,FALSE)</f>
@@ -69295,7 +69297,7 @@
     </row>
     <row r="69" spans="1:21">
       <c r="A69" s="134" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="B69" s="117" t="e">
         <f>VLOOKUP(C69,#REF!,2,FALSE)</f>
@@ -69323,7 +69325,7 @@
         <v>77</v>
       </c>
       <c r="J69" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K69" s="134" t="s">
         <v>334</v>
@@ -69361,7 +69363,7 @@
     </row>
     <row r="70" spans="1:21">
       <c r="A70" s="134" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="B70" s="117" t="e">
         <f>VLOOKUP(C70,#REF!,2,FALSE)</f>
@@ -69427,7 +69429,7 @@
     </row>
     <row r="71" spans="1:21">
       <c r="A71" s="134" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="B71" s="117" t="e">
         <f>VLOOKUP(C71,#REF!,2,FALSE)</f>
@@ -69493,7 +69495,7 @@
     </row>
     <row r="72" spans="1:21">
       <c r="A72" s="134" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="B72" s="117" t="e">
         <f>VLOOKUP(C72,#REF!,2,FALSE)</f>
@@ -69521,7 +69523,7 @@
         <v>77</v>
       </c>
       <c r="J72" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="K72" s="134" t="s">
         <v>1714</v>
@@ -69551,7 +69553,7 @@
         <v>77</v>
       </c>
       <c r="T72" s="134" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="U72" s="134" t="s">
         <v>334</v>
@@ -69559,7 +69561,7 @@
     </row>
     <row r="73" spans="1:21">
       <c r="A73" s="134" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="B73" s="117" t="e">
         <f>VLOOKUP(C73,#REF!,2,FALSE)</f>
@@ -69625,7 +69627,7 @@
     </row>
     <row r="74" spans="1:21">
       <c r="A74" s="134" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="B74" s="117" t="e">
         <f>VLOOKUP(C74,#REF!,2,FALSE)</f>
@@ -69653,7 +69655,7 @@
         <v>77</v>
       </c>
       <c r="J74" s="134" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="K74" s="134" t="s">
         <v>334</v>
@@ -69691,7 +69693,7 @@
     </row>
     <row r="75" spans="1:21">
       <c r="A75" s="134" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B75" s="117" t="e">
         <f>VLOOKUP(C75,#REF!,2,FALSE)</f>
@@ -69757,7 +69759,7 @@
     </row>
     <row r="76" spans="1:21">
       <c r="A76" s="134" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="B76" s="117" t="e">
         <f>VLOOKUP(C76,#REF!,2,FALSE)</f>
@@ -69785,7 +69787,7 @@
         <v>1002</v>
       </c>
       <c r="J76" s="134" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="K76" s="134" t="s">
         <v>334</v>
@@ -69812,7 +69814,7 @@
         <v>545</v>
       </c>
       <c r="S76" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="T76" s="134" t="s">
         <v>2009</v>
@@ -69823,7 +69825,7 @@
     </row>
     <row r="77" spans="1:21">
       <c r="A77" s="134" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B77" s="117" t="e">
         <f>VLOOKUP(C77,#REF!,2,FALSE)</f>
@@ -69851,7 +69853,7 @@
         <v>1667</v>
       </c>
       <c r="J77" s="134" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="K77" s="134" t="s">
         <v>162</v>
@@ -69889,7 +69891,7 @@
     </row>
     <row r="78" spans="1:21">
       <c r="A78" s="134" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B78" s="117" t="e">
         <f>VLOOKUP(C78,#REF!,2,FALSE)</f>
@@ -69955,7 +69957,7 @@
     </row>
     <row r="79" spans="1:21">
       <c r="A79" s="134" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B79" s="117" t="e">
         <f>VLOOKUP(C79,#REF!,2,FALSE)</f>
@@ -70021,7 +70023,7 @@
     </row>
     <row r="80" spans="1:21">
       <c r="A80" s="134" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="B80" s="117" t="e">
         <f>VLOOKUP(C80,#REF!,2,FALSE)</f>
@@ -70087,7 +70089,7 @@
     </row>
     <row r="81" spans="1:21">
       <c r="A81" s="134" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B81" s="117" t="e">
         <f>VLOOKUP(C81,#REF!,2,FALSE)</f>
@@ -70153,7 +70155,7 @@
     </row>
     <row r="82" spans="1:21">
       <c r="A82" s="134" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B82" s="117" t="e">
         <f>VLOOKUP(C82,#REF!,2,FALSE)</f>
@@ -70219,7 +70221,7 @@
     </row>
     <row r="83" spans="1:21">
       <c r="A83" s="134" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B83" s="117" t="e">
         <f>VLOOKUP(C83,#REF!,2,FALSE)</f>
@@ -70285,7 +70287,7 @@
     </row>
     <row r="84" spans="1:21">
       <c r="A84" s="134" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="B84" s="117" t="e">
         <f>VLOOKUP(C84,#REF!,2,FALSE)</f>
@@ -70351,7 +70353,7 @@
     </row>
     <row r="85" spans="1:21">
       <c r="A85" s="134" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="B85" s="117" t="e">
         <f>VLOOKUP(C85,#REF!,2,FALSE)</f>
@@ -70379,7 +70381,7 @@
         <v>77</v>
       </c>
       <c r="J85" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="K85" s="134" t="s">
         <v>599</v>
@@ -70417,7 +70419,7 @@
     </row>
     <row r="86" spans="1:21">
       <c r="A86" s="134" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="B86" s="117" t="e">
         <f>VLOOKUP(C86,#REF!,2,FALSE)</f>
@@ -70451,7 +70453,7 @@
         <v>1500</v>
       </c>
       <c r="L86" s="117" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="M86" s="139">
         <v>169</v>
@@ -70483,7 +70485,7 @@
     </row>
     <row r="87" spans="1:21">
       <c r="A87" s="134" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="B87" s="117" t="e">
         <f>VLOOKUP(C87,#REF!,2,FALSE)</f>
@@ -70549,7 +70551,7 @@
     </row>
     <row r="88" spans="1:21">
       <c r="A88" s="134" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="B88" s="117" t="e">
         <f>VLOOKUP(C88,#REF!,2,FALSE)</f>
@@ -70615,7 +70617,7 @@
     </row>
     <row r="89" spans="1:21">
       <c r="A89" s="134" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B89" s="117" t="e">
         <f>VLOOKUP(C89,#REF!,2,FALSE)</f>
@@ -70681,7 +70683,7 @@
     </row>
     <row r="90" spans="1:21">
       <c r="A90" s="134" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B90" s="117" t="e">
         <f>VLOOKUP(C90,#REF!,2,FALSE)</f>
@@ -70747,7 +70749,7 @@
     </row>
     <row r="91" spans="1:21">
       <c r="A91" s="134" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="B91" s="117" t="e">
         <f>VLOOKUP(C91,#REF!,2,FALSE)</f>
@@ -70805,7 +70807,7 @@
         <v>162</v>
       </c>
       <c r="T91" s="134" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="U91" s="134" t="s">
         <v>1793</v>
@@ -70813,7 +70815,7 @@
     </row>
     <row r="92" spans="1:21">
       <c r="A92" s="134" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="B92" s="117" t="e">
         <f>VLOOKUP(C92,#REF!,2,FALSE)</f>
@@ -70879,7 +70881,7 @@
     </row>
     <row r="93" spans="1:21">
       <c r="A93" s="134" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="B93" s="117" t="e">
         <f>VLOOKUP(C93,Weapon!A1:Z258,2,FALSE)</f>
@@ -70910,7 +70912,7 @@
         <v>487</v>
       </c>
       <c r="K93" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="L93" s="117" t="s">
         <v>159</v>
@@ -70945,7 +70947,7 @@
     </row>
     <row r="94" spans="1:21">
       <c r="A94" s="134" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="B94" s="117" t="e">
         <f>VLOOKUP(C94,#REF!,2,FALSE)</f>
@@ -70955,7 +70957,7 @@
         <v>184</v>
       </c>
       <c r="D94" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E94" s="134" t="s">
         <v>77</v>
@@ -70985,7 +70987,7 @@
         <v>185</v>
       </c>
       <c r="N94" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O94" s="134" t="s">
         <v>77</v>
@@ -71011,7 +71013,7 @@
     </row>
     <row r="95" spans="1:21">
       <c r="A95" s="134" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="B95" s="117" t="e">
         <f>VLOOKUP(C95,#REF!,2,FALSE)</f>
@@ -71021,7 +71023,7 @@
         <v>186</v>
       </c>
       <c r="D95" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E95" s="134" t="s">
         <v>77</v>
@@ -71042,16 +71044,16 @@
         <v>1826</v>
       </c>
       <c r="K95" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="L95" s="117" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="M95" s="139">
         <v>187</v>
       </c>
       <c r="N95" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O95" s="134" t="s">
         <v>77</v>
@@ -71077,7 +71079,7 @@
     </row>
     <row r="96" spans="1:21">
       <c r="A96" s="134" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="B96" s="117" t="e">
         <f>VLOOKUP(C96,#REF!,2,FALSE)</f>
@@ -71117,7 +71119,7 @@
         <v>189</v>
       </c>
       <c r="N96" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O96" s="134" t="s">
         <v>77</v>
@@ -71143,7 +71145,7 @@
     </row>
     <row r="97" spans="1:21">
       <c r="A97" s="134" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="B97" s="117" t="e">
         <f>VLOOKUP(C97,#REF!,2,FALSE)</f>
@@ -71168,7 +71170,7 @@
         <v>1678</v>
       </c>
       <c r="I97" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="J97" s="134" t="s">
         <v>1784</v>
@@ -71209,7 +71211,7 @@
     </row>
     <row r="98" spans="1:21">
       <c r="A98" s="134" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B98" s="117" t="e">
         <f>VLOOKUP(C98,#REF!,2,FALSE)</f>
@@ -71264,7 +71266,7 @@
         <v>1678</v>
       </c>
       <c r="S98" s="134" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="T98" s="134" t="s">
         <v>2042</v>
@@ -71275,7 +71277,7 @@
     </row>
     <row r="99" spans="1:21">
       <c r="A99" s="134" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="B99" s="117" t="e">
         <f>VLOOKUP(C99,#REF!,2,FALSE)</f>
@@ -71341,7 +71343,7 @@
     </row>
     <row r="100" spans="1:21">
       <c r="A100" s="134" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="B100" s="117" t="e">
         <f>VLOOKUP(C100,#REF!,2,FALSE)</f>
@@ -71407,7 +71409,7 @@
     </row>
     <row r="101" spans="1:21">
       <c r="A101" s="134" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="B101" s="117" t="e">
         <f>VLOOKUP(C101,#REF!,2,FALSE)</f>
@@ -71473,7 +71475,7 @@
     </row>
     <row r="102" spans="1:21">
       <c r="A102" s="134" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="B102" s="117" t="e">
         <f>VLOOKUP(C102,#REF!,2,FALSE)</f>
@@ -71539,7 +71541,7 @@
     </row>
     <row r="103" spans="1:21">
       <c r="A103" s="134" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B103" s="117" t="e">
         <f>VLOOKUP(C103,#REF!,2,FALSE)</f>
@@ -71605,7 +71607,7 @@
     </row>
     <row r="104" spans="1:21">
       <c r="A104" s="134" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="B104" s="117" t="e">
         <f>VLOOKUP(C104,#REF!,2,FALSE)</f>
@@ -71671,7 +71673,7 @@
     </row>
     <row r="105" spans="1:21">
       <c r="A105" s="134" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="B105" s="117" t="e">
         <f>VLOOKUP(C105,#REF!,2,FALSE)</f>
@@ -71737,7 +71739,7 @@
     </row>
     <row r="106" spans="1:21">
       <c r="A106" s="134" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="B106" s="117" t="e">
         <f>VLOOKUP(C106,#REF!,2,FALSE)</f>
@@ -71803,7 +71805,7 @@
     </row>
     <row r="107" spans="1:21">
       <c r="A107" s="134" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="B107" s="117" t="e">
         <f>VLOOKUP(C107,#REF!,2,FALSE)</f>
@@ -71869,7 +71871,7 @@
     </row>
     <row r="108" spans="1:21">
       <c r="A108" s="134" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="B108" s="117" t="e">
         <f>VLOOKUP(C108,#REF!,2,FALSE)</f>
@@ -71935,7 +71937,7 @@
     </row>
     <row r="109" spans="1:21">
       <c r="A109" s="134" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B109" s="117" t="e">
         <f>VLOOKUP(C109,#REF!,2,FALSE)</f>
@@ -72001,7 +72003,7 @@
     </row>
     <row r="110" spans="1:21">
       <c r="A110" s="134" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="B110" s="117" t="e">
         <f>VLOOKUP(C110,#REF!,2,FALSE)</f>
@@ -72041,7 +72043,7 @@
         <v>217</v>
       </c>
       <c r="N110" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O110" s="134" t="s">
         <v>77</v>
@@ -72059,7 +72061,7 @@
         <v>77</v>
       </c>
       <c r="T110" s="134" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="U110" s="134" t="s">
         <v>36</v>
@@ -72067,7 +72069,7 @@
     </row>
     <row r="111" spans="1:21">
       <c r="A111" s="134" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B111" s="117" t="e">
         <f>VLOOKUP(C111,#REF!,2,FALSE)</f>
@@ -72077,7 +72079,7 @@
         <v>218</v>
       </c>
       <c r="D111" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E111" s="134" t="s">
         <v>77</v>
@@ -72107,7 +72109,7 @@
         <v>219</v>
       </c>
       <c r="N111" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O111" s="134" t="s">
         <v>77</v>
@@ -72133,7 +72135,7 @@
     </row>
     <row r="112" spans="1:21">
       <c r="A112" s="134" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B112" s="117" t="e">
         <f>VLOOKUP(C112,#REF!,2,FALSE)</f>
@@ -72143,7 +72145,7 @@
         <v>220</v>
       </c>
       <c r="D112" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E112" s="134" t="s">
         <v>77</v>
@@ -72164,7 +72166,7 @@
         <v>1684</v>
       </c>
       <c r="K112" s="134" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="L112" s="117" t="s">
         <v>202</v>
@@ -72173,7 +72175,7 @@
         <v>221</v>
       </c>
       <c r="N112" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O112" s="134" t="s">
         <v>77</v>
@@ -72199,7 +72201,7 @@
     </row>
     <row r="113" spans="1:21">
       <c r="A113" s="134" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B113" s="117" t="e">
         <f>VLOOKUP(C113,#REF!,2,FALSE)</f>
@@ -72209,7 +72211,7 @@
         <v>222</v>
       </c>
       <c r="D113" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E113" s="134" t="s">
         <v>77</v>
@@ -72239,7 +72241,7 @@
         <v>223</v>
       </c>
       <c r="N113" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O113" s="134" t="s">
         <v>77</v>
@@ -72265,7 +72267,7 @@
     </row>
     <row r="114" spans="1:21">
       <c r="A114" s="134" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B114" s="117" t="e">
         <f>VLOOKUP(C114,#REF!,2,FALSE)</f>
@@ -72275,7 +72277,7 @@
         <v>224</v>
       </c>
       <c r="D114" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E114" s="134" t="s">
         <v>77</v>
@@ -72305,7 +72307,7 @@
         <v>225</v>
       </c>
       <c r="N114" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="O114" s="134" t="s">
         <v>77</v>
@@ -72331,7 +72333,7 @@
     </row>
     <row r="115" spans="1:21">
       <c r="A115" s="134" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B115" s="117" t="e">
         <f>VLOOKUP(C115,#REF!,2,FALSE)</f>
@@ -72341,7 +72343,7 @@
         <v>226</v>
       </c>
       <c r="D115" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E115" s="134" t="s">
         <v>77</v>
@@ -72397,7 +72399,7 @@
     </row>
     <row r="116" spans="1:21">
       <c r="A116" s="134" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="B116" s="117" t="e">
         <f>VLOOKUP(C116,#REF!,2,FALSE)</f>
@@ -72463,7 +72465,7 @@
     </row>
     <row r="117" spans="1:21">
       <c r="A117" s="134" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="B117" s="117" t="e">
         <f>VLOOKUP(C117,#REF!,2,FALSE)</f>
@@ -72479,7 +72481,7 @@
         <v>77</v>
       </c>
       <c r="F117" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G117" s="134" t="s">
         <v>77</v>
@@ -72509,7 +72511,7 @@
         <v>77</v>
       </c>
       <c r="P117" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q117" s="134" t="s">
         <v>77</v>
@@ -72529,7 +72531,7 @@
     </row>
     <row r="118" spans="1:21">
       <c r="A118" s="134" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="B118" s="117" t="e">
         <f>VLOOKUP(C118,#REF!,2,FALSE)</f>
@@ -72545,7 +72547,7 @@
         <v>77</v>
       </c>
       <c r="F118" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G118" s="134" t="s">
         <v>77</v>
@@ -72575,7 +72577,7 @@
         <v>77</v>
       </c>
       <c r="P118" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q118" s="134" t="s">
         <v>77</v>
@@ -72595,7 +72597,7 @@
     </row>
     <row r="119" spans="1:21">
       <c r="A119" s="134" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="B119" s="117" t="e">
         <f>VLOOKUP(C119,#REF!,2,FALSE)</f>
@@ -72611,7 +72613,7 @@
         <v>77</v>
       </c>
       <c r="F119" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G119" s="134" t="s">
         <v>77</v>
@@ -72641,7 +72643,7 @@
         <v>77</v>
       </c>
       <c r="P119" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q119" s="134" t="s">
         <v>77</v>
@@ -72661,7 +72663,7 @@
     </row>
     <row r="120" spans="1:21">
       <c r="A120" s="134" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B120" s="117" t="e">
         <f>VLOOKUP(C120,#REF!,2,FALSE)</f>
@@ -72677,7 +72679,7 @@
         <v>77</v>
       </c>
       <c r="F120" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G120" s="134" t="s">
         <v>77</v>
@@ -72707,7 +72709,7 @@
         <v>77</v>
       </c>
       <c r="P120" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q120" s="134" t="s">
         <v>77</v>
@@ -72727,7 +72729,7 @@
     </row>
     <row r="121" spans="1:21">
       <c r="A121" s="134" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="B121" s="117" t="e">
         <f>VLOOKUP(C121,#REF!,2,FALSE)</f>
@@ -72743,7 +72745,7 @@
         <v>77</v>
       </c>
       <c r="F121" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="G121" s="134" t="s">
         <v>77</v>
@@ -72773,7 +72775,7 @@
         <v>77</v>
       </c>
       <c r="P121" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q121" s="134" t="s">
         <v>77</v>
@@ -72793,7 +72795,7 @@
     </row>
     <row r="122" spans="1:21">
       <c r="A122" s="134" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B122" s="117" t="e">
         <f>VLOOKUP(C122,#REF!,2,FALSE)</f>
@@ -72859,7 +72861,7 @@
     </row>
     <row r="123" spans="1:21">
       <c r="A123" s="134" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="B123" s="117" t="e">
         <f>VLOOKUP(C123,#REF!,2,FALSE)</f>
@@ -72925,7 +72927,7 @@
     </row>
     <row r="124" spans="1:21">
       <c r="A124" s="134" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="B124" s="117" t="e">
         <f>VLOOKUP(C124,#REF!,2,FALSE)</f>
@@ -72971,7 +72973,7 @@
         <v>77</v>
       </c>
       <c r="P124" s="134" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="Q124" s="134" t="s">
         <v>77</v>
@@ -72980,7 +72982,7 @@
         <v>77</v>
       </c>
       <c r="S124" s="134" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="T124" s="134" t="s">
         <v>460</v>
@@ -72991,7 +72993,7 @@
     </row>
     <row r="125" spans="1:21">
       <c r="A125" s="134" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="B125" s="117" t="e">
         <f>VLOOKUP(C125,#REF!,2,FALSE)</f>
@@ -73001,7 +73003,7 @@
         <v>246</v>
       </c>
       <c r="D125" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E125" s="134" t="s">
         <v>77</v>
@@ -73043,10 +73045,10 @@
         <v>599</v>
       </c>
       <c r="R125" s="134" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="S125" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T125" s="134" t="s">
         <v>460</v>
@@ -73057,7 +73059,7 @@
     </row>
     <row r="126" spans="1:21">
       <c r="A126" s="134" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="B126" s="117" t="e">
         <f>VLOOKUP(C126,#REF!,2,FALSE)</f>
@@ -73123,7 +73125,7 @@
     </row>
     <row r="127" spans="1:21">
       <c r="A127" s="134" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="B127" s="117" t="e">
         <f>VLOOKUP(C127,#REF!,2,FALSE)</f>
@@ -73133,7 +73135,7 @@
         <v>250</v>
       </c>
       <c r="D127" s="134" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="E127" s="134" t="s">
         <v>77</v>
@@ -73154,7 +73156,7 @@
         <v>1684</v>
       </c>
       <c r="K127" s="134" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="L127" s="117" t="e">
         <v>#N/A</v>
@@ -73189,7 +73191,7 @@
     </row>
     <row r="128" spans="1:21">
       <c r="A128" s="134" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="B128" s="117" t="e">
         <f>VLOOKUP(C128,#REF!,2,FALSE)</f>
@@ -73214,7 +73216,7 @@
         <v>93</v>
       </c>
       <c r="I128" s="134" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="J128" s="134" t="s">
         <v>1757</v>
@@ -73255,7 +73257,7 @@
     </row>
     <row r="129" spans="1:21">
       <c r="A129" s="134" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="B129" s="117" t="e">
         <f>VLOOKUP(C129,#REF!,2,FALSE)</f>
@@ -73321,7 +73323,7 @@
     </row>
     <row r="130" spans="1:21">
       <c r="A130" s="134" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="B130" s="117" t="e">
         <f>VLOOKUP(C130,#REF!,2,FALSE)</f>
@@ -73355,7 +73357,7 @@
         <v>128</v>
       </c>
       <c r="L130" s="117" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="M130" s="139">
         <v>257</v>
@@ -73387,7 +73389,7 @@
     </row>
     <row r="131" spans="1:21">
       <c r="A131" s="134" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="B131" s="117" t="e">
         <f>VLOOKUP(C131,#REF!,2,FALSE)</f>
@@ -73421,7 +73423,7 @@
         <v>128</v>
       </c>
       <c r="L131" s="117" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="M131" s="139">
         <v>259</v>
@@ -73453,7 +73455,7 @@
     </row>
     <row r="132" spans="1:21">
       <c r="A132" s="134" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="B132" s="117" t="e">
         <f>VLOOKUP(C132,#REF!,2,FALSE)</f>
@@ -73487,7 +73489,7 @@
         <v>128</v>
       </c>
       <c r="L132" s="117" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="M132" s="139">
         <v>261</v>
@@ -73519,7 +73521,7 @@
     </row>
     <row r="133" spans="1:21">
       <c r="A133" s="134" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="B133" s="117" t="e">
         <f>VLOOKUP(C133,#REF!,2,FALSE)</f>
@@ -73553,7 +73555,7 @@
         <v>128</v>
       </c>
       <c r="L133" s="117" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="M133" s="139">
         <v>263</v>
@@ -73585,7 +73587,7 @@
     </row>
     <row r="134" spans="1:21">
       <c r="A134" s="134" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="B134" s="117" t="e">
         <f>VLOOKUP(C134,#REF!,2,FALSE)</f>
@@ -73637,10 +73639,10 @@
         <v>696</v>
       </c>
       <c r="R134" s="134" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="S134" s="134" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="T134" s="134" t="s">
         <v>460</v>
@@ -73651,7 +73653,7 @@
     </row>
     <row r="135" spans="1:21">
       <c r="A135" s="134" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="B135" s="117" t="e">
         <f>VLOOKUP(C135,#REF!,2,FALSE)</f>
@@ -73717,7 +73719,7 @@
     </row>
     <row r="136" spans="1:21">
       <c r="A136" s="134" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="B136" s="117" t="e">
         <f>VLOOKUP(C136,#REF!,2,FALSE)</f>
@@ -73783,7 +73785,7 @@
     </row>
     <row r="137" spans="1:21">
       <c r="A137" s="134" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="B137" s="117" t="e">
         <f>VLOOKUP(C137,#REF!,2,FALSE)</f>

</xml_diff>